<commit_message>
Fix typo weird spacing wikipathways names
</commit_message>
<xml_diff>
--- a/mappings/wikipathways_reactome.xlsx
+++ b/mappings/wikipathways_reactome.xlsx
@@ -713,9 +713,6 @@
     <t>Factors and pathways affecting insulin-like growth factor (IGF1)-Akt signaling</t>
   </si>
   <si>
-    <t>Farnesoid X Receptor Pathway</t>
-  </si>
-  <si>
     <t>Fas Ligand (FasL) pathway and Stress induction of Heat Shock Proteins (HSP) regulation</t>
   </si>
   <si>
@@ -2416,6 +2413,9 @@
   <si>
     <t>T-Cell antigen Receptor (TCR)  Signaling Pathway* isPartOf Immune System
 T-Cell antigen Receptor (TCR)  Signaling Pathway* isPartOf Adaptive Immune System</t>
+  </si>
+  <si>
+    <t>Farnesoid X Receptor  Pathway</t>
   </si>
 </sst>
 </file>
@@ -2782,8 +2782,8 @@
   </sheetPr>
   <dimension ref="A1:Y999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A399" zoomScale="60" workbookViewId="0">
-      <selection activeCell="C413" sqref="C413"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="60" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2803,7 +2803,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -3010,7 +3010,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -4311,13 +4311,13 @@
     </row>
     <row r="51" spans="1:25" ht="409" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>660</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>661</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>662</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="122" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="4" t="s">
-        <v>189</v>
+        <v>668</v>
       </c>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -6481,11 +6481,11 @@
     </row>
     <row r="123" spans="1:25" ht="182" x14ac:dyDescent="0.15">
       <c r="A123" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B123" s="4"/>
       <c r="C123" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
@@ -6512,13 +6512,13 @@
     </row>
     <row r="124" spans="1:25" ht="299" x14ac:dyDescent="0.15">
       <c r="A124" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B124" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B124" s="5" t="s">
+      <c r="C124" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>194</v>
       </c>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
@@ -6545,11 +6545,11 @@
     </row>
     <row r="125" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A125" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B125" s="4"/>
       <c r="C125" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
@@ -6576,11 +6576,11 @@
     </row>
     <row r="126" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A126" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B126" s="4"/>
       <c r="C126" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
@@ -6607,11 +6607,11 @@
     </row>
     <row r="127" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B127" s="4"/>
       <c r="C127" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
@@ -6638,11 +6638,11 @@
     </row>
     <row r="128" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A128" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B128" s="4"/>
       <c r="C128" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
@@ -6669,11 +6669,11 @@
     </row>
     <row r="129" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A129" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B129" s="4"/>
       <c r="C129" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
@@ -6700,11 +6700,11 @@
     </row>
     <row r="130" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A130" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B130" s="4"/>
       <c r="C130" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
@@ -6731,7 +6731,7 @@
     </row>
     <row r="131" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A131" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -6760,11 +6760,11 @@
     </row>
     <row r="132" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A132" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B132" s="4"/>
       <c r="C132" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
@@ -6791,7 +6791,7 @@
     </row>
     <row r="133" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A133" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -6820,7 +6820,7 @@
     </row>
     <row r="134" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A134" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -6849,7 +6849,7 @@
     </row>
     <row r="135" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -6878,11 +6878,11 @@
     </row>
     <row r="136" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A136" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B136" s="4"/>
       <c r="C136" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
@@ -6909,11 +6909,11 @@
     </row>
     <row r="137" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A137" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B137" s="4"/>
       <c r="C137" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
@@ -6940,13 +6940,13 @@
     </row>
     <row r="138" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A138" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B138" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="C138" s="4" t="s">
         <v>218</v>
-      </c>
-      <c r="C138" s="4" t="s">
-        <v>219</v>
       </c>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
@@ -6973,10 +6973,10 @@
     </row>
     <row r="139" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A139" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B139" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="B139" s="4" t="s">
-        <v>221</v>
       </c>
       <c r="C139" s="4"/>
       <c r="D139" s="2"/>
@@ -7004,10 +7004,10 @@
     </row>
     <row r="140" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A140" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B140" s="4" t="s">
         <v>222</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>223</v>
       </c>
       <c r="C140" s="4"/>
       <c r="D140" s="2"/>
@@ -7035,10 +7035,10 @@
     </row>
     <row r="141" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A141" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C141" s="4"/>
       <c r="D141" s="2"/>
@@ -7066,11 +7066,11 @@
     </row>
     <row r="142" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A142" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B142" s="4"/>
       <c r="C142" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
@@ -7097,10 +7097,10 @@
     </row>
     <row r="143" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A143" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B143" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="B143" s="4" t="s">
-        <v>228</v>
       </c>
       <c r="C143" s="4"/>
       <c r="D143" s="2"/>
@@ -7128,11 +7128,11 @@
     </row>
     <row r="144" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A144" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B144" s="4"/>
       <c r="C144" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
@@ -7159,7 +7159,7 @@
     </row>
     <row r="145" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A145" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
@@ -7188,7 +7188,7 @@
     </row>
     <row r="146" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A146" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
@@ -7217,7 +7217,7 @@
     </row>
     <row r="147" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A147" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
@@ -7246,7 +7246,7 @@
     </row>
     <row r="148" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A148" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
@@ -7275,11 +7275,11 @@
     </row>
     <row r="149" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A149" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B149" s="4"/>
       <c r="C149" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
@@ -7306,11 +7306,11 @@
     </row>
     <row r="150" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A150" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B150" s="4"/>
       <c r="C150" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
@@ -7337,11 +7337,11 @@
     </row>
     <row r="151" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A151" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B151" s="4"/>
       <c r="C151" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
@@ -7368,11 +7368,11 @@
     </row>
     <row r="152" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A152" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B152" s="4"/>
       <c r="C152" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
@@ -7399,10 +7399,10 @@
     </row>
     <row r="153" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A153" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B153" s="4" t="s">
         <v>243</v>
-      </c>
-      <c r="B153" s="4" t="s">
-        <v>244</v>
       </c>
       <c r="C153" s="4"/>
       <c r="D153" s="2"/>
@@ -7430,11 +7430,11 @@
     </row>
     <row r="154" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A154" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B154" s="4"/>
       <c r="C154" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
@@ -7461,10 +7461,10 @@
     </row>
     <row r="155" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A155" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B155" s="4" t="s">
         <v>247</v>
-      </c>
-      <c r="B155" s="4" t="s">
-        <v>248</v>
       </c>
       <c r="C155" s="4"/>
       <c r="D155" s="2"/>
@@ -7492,10 +7492,10 @@
     </row>
     <row r="156" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A156" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B156" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="B156" s="4" t="s">
-        <v>250</v>
       </c>
       <c r="C156" s="4"/>
       <c r="D156" s="2"/>
@@ -7523,11 +7523,11 @@
     </row>
     <row r="157" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A157" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B157" s="4"/>
       <c r="C157" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
@@ -7554,11 +7554,11 @@
     </row>
     <row r="158" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A158" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B158" s="4"/>
       <c r="C158" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
@@ -7585,7 +7585,7 @@
     </row>
     <row r="159" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
@@ -7614,11 +7614,11 @@
     </row>
     <row r="160" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A160" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B160" s="4"/>
       <c r="C160" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
@@ -7645,7 +7645,7 @@
     </row>
     <row r="161" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A161" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
@@ -7674,10 +7674,10 @@
     </row>
     <row r="162" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B162" s="4" t="s">
         <v>259</v>
-      </c>
-      <c r="B162" s="4" t="s">
-        <v>260</v>
       </c>
       <c r="C162" s="4"/>
       <c r="D162" s="2"/>
@@ -7705,7 +7705,7 @@
     </row>
     <row r="163" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
@@ -7734,7 +7734,7 @@
     </row>
     <row r="164" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A164" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
@@ -7763,10 +7763,10 @@
     </row>
     <row r="165" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B165" s="4" t="s">
         <v>263</v>
-      </c>
-      <c r="B165" s="4" t="s">
-        <v>264</v>
       </c>
       <c r="C165" s="4"/>
       <c r="D165" s="2"/>
@@ -7794,7 +7794,7 @@
     </row>
     <row r="166" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A166" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
@@ -7823,7 +7823,7 @@
     </row>
     <row r="167" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A167" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
@@ -7852,11 +7852,11 @@
     </row>
     <row r="168" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B168" s="4"/>
       <c r="C168" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
@@ -7883,7 +7883,7 @@
     </row>
     <row r="169" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A169" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
@@ -7912,11 +7912,11 @@
     </row>
     <row r="170" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A170" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B170" s="4"/>
       <c r="C170" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
@@ -7943,10 +7943,10 @@
     </row>
     <row r="171" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B171" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="B171" s="4" t="s">
-        <v>273</v>
       </c>
       <c r="C171" s="4"/>
       <c r="D171" s="2"/>
@@ -7974,7 +7974,7 @@
     </row>
     <row r="172" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A172" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
@@ -8003,7 +8003,7 @@
     </row>
     <row r="173" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A173" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
@@ -8032,7 +8032,7 @@
     </row>
     <row r="174" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A174" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
@@ -8061,7 +8061,7 @@
     </row>
     <row r="175" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A175" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
@@ -8090,7 +8090,7 @@
     </row>
     <row r="176" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A176" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
@@ -8119,7 +8119,7 @@
     </row>
     <row r="177" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A177" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
@@ -8148,7 +8148,7 @@
     </row>
     <row r="178" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A178" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
@@ -8177,10 +8177,10 @@
     </row>
     <row r="179" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A179" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B179" s="4" t="s">
         <v>281</v>
-      </c>
-      <c r="B179" s="4" t="s">
-        <v>282</v>
       </c>
       <c r="C179" s="4"/>
       <c r="D179" s="2"/>
@@ -8208,10 +8208,10 @@
     </row>
     <row r="180" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A180" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C180" s="4"/>
       <c r="D180" s="2"/>
@@ -8239,11 +8239,11 @@
     </row>
     <row r="181" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A181" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B181" s="4"/>
       <c r="C181" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
@@ -8270,11 +8270,11 @@
     </row>
     <row r="182" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A182" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B182" s="4"/>
       <c r="C182" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
@@ -8301,11 +8301,11 @@
     </row>
     <row r="183" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A183" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B183" s="4"/>
       <c r="C183" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
@@ -8332,10 +8332,10 @@
     </row>
     <row r="184" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A184" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B184" s="4" t="s">
         <v>290</v>
-      </c>
-      <c r="B184" s="4" t="s">
-        <v>291</v>
       </c>
       <c r="C184" s="4"/>
       <c r="D184" s="2"/>
@@ -8363,10 +8363,10 @@
     </row>
     <row r="185" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A185" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B185" s="4" t="s">
         <v>292</v>
-      </c>
-      <c r="B185" s="4" t="s">
-        <v>293</v>
       </c>
       <c r="C185" s="4"/>
       <c r="D185" s="2"/>
@@ -8394,10 +8394,10 @@
     </row>
     <row r="186" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B186" s="4" t="s">
         <v>294</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>295</v>
       </c>
       <c r="C186" s="4"/>
       <c r="D186" s="2"/>
@@ -8425,11 +8425,11 @@
     </row>
     <row r="187" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A187" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B187" s="4"/>
       <c r="C187" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
@@ -8456,10 +8456,10 @@
     </row>
     <row r="188" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A188" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B188" s="4" t="s">
         <v>298</v>
-      </c>
-      <c r="B188" s="4" t="s">
-        <v>299</v>
       </c>
       <c r="C188" s="4"/>
       <c r="D188" s="2"/>
@@ -8487,7 +8487,7 @@
     </row>
     <row r="189" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A189" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
@@ -8516,11 +8516,11 @@
     </row>
     <row r="190" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A190" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B190" s="4"/>
       <c r="C190" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
@@ -8547,11 +8547,11 @@
     </row>
     <row r="191" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A191" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B191" s="4"/>
       <c r="C191" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
@@ -8578,7 +8578,7 @@
     </row>
     <row r="192" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A192" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
@@ -8607,7 +8607,7 @@
     </row>
     <row r="193" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A193" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B193" s="4"/>
       <c r="C193" s="4"/>
@@ -8636,11 +8636,11 @@
     </row>
     <row r="194" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A194" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B194" s="4"/>
       <c r="C194" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
@@ -8667,11 +8667,11 @@
     </row>
     <row r="195" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A195" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B195" s="4"/>
       <c r="C195" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
@@ -8698,7 +8698,7 @@
     </row>
     <row r="196" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A196" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B196" s="4"/>
       <c r="C196" s="4"/>
@@ -8727,11 +8727,11 @@
     </row>
     <row r="197" spans="1:25" ht="130" x14ac:dyDescent="0.15">
       <c r="A197" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B197" s="4"/>
       <c r="C197" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
@@ -8758,11 +8758,11 @@
     </row>
     <row r="198" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A198" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B198" s="4"/>
       <c r="C198" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D198" s="2"/>
       <c r="E198" s="2"/>
@@ -8789,7 +8789,7 @@
     </row>
     <row r="199" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A199" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B199" s="4"/>
       <c r="C199" s="4"/>
@@ -8818,11 +8818,11 @@
     </row>
     <row r="200" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A200" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B200" s="4"/>
       <c r="C200" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
@@ -8849,11 +8849,11 @@
     </row>
     <row r="201" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A201" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B201" s="4"/>
       <c r="C201" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
@@ -8880,11 +8880,11 @@
     </row>
     <row r="202" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A202" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B202" s="4"/>
       <c r="C202" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D202" s="2"/>
       <c r="E202" s="2"/>
@@ -8911,7 +8911,7 @@
     </row>
     <row r="203" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A203" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B203" s="4"/>
       <c r="C203" s="4"/>
@@ -8940,11 +8940,11 @@
     </row>
     <row r="204" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A204" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B204" s="4"/>
       <c r="C204" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
@@ -8971,11 +8971,11 @@
     </row>
     <row r="205" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A205" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B205" s="4"/>
       <c r="C205" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D205" s="2"/>
       <c r="E205" s="2"/>
@@ -9002,11 +9002,11 @@
     </row>
     <row r="206" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A206" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B206" s="4"/>
       <c r="C206" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D206" s="2"/>
       <c r="E206" s="2"/>
@@ -9033,11 +9033,11 @@
     </row>
     <row r="207" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A207" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B207" s="4"/>
       <c r="C207" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
@@ -9064,11 +9064,11 @@
     </row>
     <row r="208" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A208" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B208" s="4"/>
       <c r="C208" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
@@ -9095,10 +9095,10 @@
     </row>
     <row r="209" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A209" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="B209" s="4" t="s">
         <v>334</v>
-      </c>
-      <c r="B209" s="4" t="s">
-        <v>335</v>
       </c>
       <c r="C209" s="4"/>
       <c r="D209" s="2"/>
@@ -9126,11 +9126,11 @@
     </row>
     <row r="210" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A210" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B210" s="4"/>
       <c r="C210" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D210" s="2"/>
       <c r="E210" s="2"/>
@@ -9157,10 +9157,10 @@
     </row>
     <row r="211" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A211" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="B211" s="4" t="s">
         <v>338</v>
-      </c>
-      <c r="B211" s="4" t="s">
-        <v>339</v>
       </c>
       <c r="C211" s="4"/>
       <c r="D211" s="2"/>
@@ -9188,11 +9188,11 @@
     </row>
     <row r="212" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A212" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B212" s="4"/>
       <c r="C212" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D212" s="2"/>
       <c r="E212" s="2"/>
@@ -9219,7 +9219,7 @@
     </row>
     <row r="213" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A213" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B213" s="4"/>
       <c r="C213" s="4"/>
@@ -9248,7 +9248,7 @@
     </row>
     <row r="214" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A214" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B214" s="4"/>
       <c r="C214" s="4"/>
@@ -9277,7 +9277,7 @@
     </row>
     <row r="215" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A215" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B215" s="4"/>
       <c r="C215" s="4"/>
@@ -9306,10 +9306,10 @@
     </row>
     <row r="216" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A216" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="B216" s="4" t="s">
         <v>345</v>
-      </c>
-      <c r="B216" s="4" t="s">
-        <v>346</v>
       </c>
       <c r="C216" s="4"/>
       <c r="D216" s="2"/>
@@ -9337,10 +9337,10 @@
     </row>
     <row r="217" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A217" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B217" s="4" t="s">
         <v>347</v>
-      </c>
-      <c r="B217" s="4" t="s">
-        <v>348</v>
       </c>
       <c r="C217" s="4"/>
       <c r="D217" s="2"/>
@@ -9368,7 +9368,7 @@
     </row>
     <row r="218" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A218" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B218" s="4"/>
       <c r="C218" s="4"/>
@@ -9397,7 +9397,7 @@
     </row>
     <row r="219" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A219" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B219" s="4"/>
       <c r="C219" s="4"/>
@@ -9426,11 +9426,11 @@
     </row>
     <row r="220" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A220" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B220" s="4"/>
       <c r="C220" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
@@ -9457,11 +9457,11 @@
     </row>
     <row r="221" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A221" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B221" s="4"/>
       <c r="C221" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
@@ -9488,7 +9488,7 @@
     </row>
     <row r="222" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A222" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B222" s="4"/>
       <c r="C222" s="4"/>
@@ -9517,7 +9517,7 @@
     </row>
     <row r="223" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A223" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B223" s="4"/>
       <c r="C223" s="4"/>
@@ -9546,11 +9546,11 @@
     </row>
     <row r="224" spans="1:25" ht="130" x14ac:dyDescent="0.15">
       <c r="A224" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B224" s="4"/>
       <c r="C224" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
@@ -9577,11 +9577,11 @@
     </row>
     <row r="225" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A225" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B225" s="4"/>
       <c r="C225" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D225" s="2"/>
       <c r="E225" s="2"/>
@@ -9608,7 +9608,7 @@
     </row>
     <row r="226" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A226" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B226" s="4"/>
       <c r="C226" s="4"/>
@@ -9637,7 +9637,7 @@
     </row>
     <row r="227" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A227" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B227" s="4"/>
       <c r="C227" s="4"/>
@@ -9666,13 +9666,13 @@
     </row>
     <row r="228" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A228" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B228" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="B228" s="4" t="s">
+      <c r="C228" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="C228" s="4" t="s">
-        <v>365</v>
       </c>
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
@@ -9699,10 +9699,10 @@
     </row>
     <row r="229" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A229" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B229" s="4" t="s">
         <v>366</v>
-      </c>
-      <c r="B229" s="4" t="s">
-        <v>367</v>
       </c>
       <c r="C229" s="4"/>
       <c r="D229" s="2"/>
@@ -9730,7 +9730,7 @@
     </row>
     <row r="230" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A230" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B230" s="4"/>
       <c r="C230" s="4"/>
@@ -9759,11 +9759,11 @@
     </row>
     <row r="231" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A231" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B231" s="4"/>
       <c r="C231" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D231" s="2"/>
       <c r="E231" s="2"/>
@@ -9790,10 +9790,10 @@
     </row>
     <row r="232" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A232" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B232" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="B232" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="C232" s="4"/>
       <c r="D232" s="2"/>
@@ -9821,11 +9821,11 @@
     </row>
     <row r="233" spans="1:25" ht="221" x14ac:dyDescent="0.15">
       <c r="A233" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B233" s="4"/>
       <c r="C233" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
@@ -9852,11 +9852,11 @@
     </row>
     <row r="234" spans="1:25" ht="273" x14ac:dyDescent="0.15">
       <c r="A234" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B234" s="4"/>
       <c r="C234" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
@@ -9883,11 +9883,11 @@
     </row>
     <row r="235" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A235" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B235" s="4"/>
       <c r="C235" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D235" s="2"/>
       <c r="E235" s="2"/>
@@ -9914,11 +9914,11 @@
     </row>
     <row r="236" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A236" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B236" s="4"/>
       <c r="C236" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D236" s="2"/>
       <c r="E236" s="2"/>
@@ -9945,7 +9945,7 @@
     </row>
     <row r="237" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A237" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B237" s="4"/>
       <c r="C237" s="4"/>
@@ -9974,11 +9974,11 @@
     </row>
     <row r="238" spans="1:25" ht="169" x14ac:dyDescent="0.15">
       <c r="A238" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B238" s="4"/>
       <c r="C238" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
@@ -10005,7 +10005,7 @@
     </row>
     <row r="239" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A239" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B239" s="4"/>
       <c r="C239" s="4"/>
@@ -10034,11 +10034,11 @@
     </row>
     <row r="240" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A240" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B240" s="4"/>
       <c r="C240" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
@@ -10065,11 +10065,11 @@
     </row>
     <row r="241" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A241" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B241" s="4"/>
       <c r="C241" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D241" s="2"/>
       <c r="E241" s="2"/>
@@ -10096,11 +10096,11 @@
     </row>
     <row r="242" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A242" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B242" s="4"/>
       <c r="C242" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D242" s="2"/>
       <c r="E242" s="2"/>
@@ -10127,7 +10127,7 @@
     </row>
     <row r="243" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A243" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B243" s="4"/>
       <c r="C243" s="4"/>
@@ -10156,7 +10156,7 @@
     </row>
     <row r="244" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A244" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B244" s="4"/>
       <c r="C244" s="4"/>
@@ -10185,7 +10185,7 @@
     </row>
     <row r="245" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A245" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B245" s="4"/>
       <c r="C245" s="4"/>
@@ -10214,11 +10214,11 @@
     </row>
     <row r="246" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A246" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B246" s="4"/>
       <c r="C246" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D246" s="2"/>
       <c r="E246" s="2"/>
@@ -10245,7 +10245,7 @@
     </row>
     <row r="247" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A247" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B247" s="4"/>
       <c r="C247" s="4"/>
@@ -10274,11 +10274,11 @@
     </row>
     <row r="248" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A248" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B248" s="4"/>
       <c r="C248" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D248" s="2"/>
       <c r="E248" s="2"/>
@@ -10305,7 +10305,7 @@
     </row>
     <row r="249" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A249" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B249" s="4"/>
       <c r="C249" s="4"/>
@@ -10334,7 +10334,7 @@
     </row>
     <row r="250" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A250" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B250" s="4"/>
       <c r="C250" s="4"/>
@@ -10363,11 +10363,11 @@
     </row>
     <row r="251" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A251" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B251" s="4"/>
       <c r="C251" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D251" s="2"/>
       <c r="E251" s="2"/>
@@ -10394,7 +10394,7 @@
     </row>
     <row r="252" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A252" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B252" s="4"/>
       <c r="C252" s="4"/>
@@ -10423,11 +10423,11 @@
     </row>
     <row r="253" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A253" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B253" s="4"/>
       <c r="C253" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D253" s="2"/>
       <c r="E253" s="2"/>
@@ -10454,11 +10454,11 @@
     </row>
     <row r="254" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A254" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B254" s="4"/>
       <c r="C254" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D254" s="2"/>
       <c r="E254" s="2"/>
@@ -10485,10 +10485,10 @@
     </row>
     <row r="255" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A255" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="B255" s="4" t="s">
         <v>408</v>
-      </c>
-      <c r="B255" s="4" t="s">
-        <v>409</v>
       </c>
       <c r="C255" s="4"/>
       <c r="D255" s="2"/>
@@ -10516,10 +10516,10 @@
     </row>
     <row r="256" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A256" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="B256" s="4" t="s">
         <v>410</v>
-      </c>
-      <c r="B256" s="4" t="s">
-        <v>411</v>
       </c>
       <c r="C256" s="4"/>
       <c r="D256" s="2"/>
@@ -10547,11 +10547,11 @@
     </row>
     <row r="257" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A257" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B257" s="4"/>
       <c r="C257" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D257" s="2"/>
       <c r="E257" s="2"/>
@@ -10578,11 +10578,11 @@
     </row>
     <row r="258" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A258" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B258" s="4"/>
       <c r="C258" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D258" s="2"/>
       <c r="E258" s="2"/>
@@ -10609,7 +10609,7 @@
     </row>
     <row r="259" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A259" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B259" s="4"/>
       <c r="C259" s="4"/>
@@ -10638,10 +10638,10 @@
     </row>
     <row r="260" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A260" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="B260" s="4" t="s">
         <v>417</v>
-      </c>
-      <c r="B260" s="4" t="s">
-        <v>418</v>
       </c>
       <c r="C260" s="4"/>
       <c r="D260" s="2"/>
@@ -10669,7 +10669,7 @@
     </row>
     <row r="261" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A261" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B261" s="4"/>
       <c r="C261" s="4"/>
@@ -10698,7 +10698,7 @@
     </row>
     <row r="262" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A262" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B262" s="4"/>
       <c r="C262" s="4"/>
@@ -10727,11 +10727,11 @@
     </row>
     <row r="263" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A263" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B263" s="4"/>
       <c r="C263" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D263" s="2"/>
       <c r="E263" s="2"/>
@@ -10758,11 +10758,11 @@
     </row>
     <row r="264" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A264" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B264" s="4"/>
       <c r="C264" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D264" s="2"/>
       <c r="E264" s="2"/>
@@ -10789,11 +10789,11 @@
     </row>
     <row r="265" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A265" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B265" s="4"/>
       <c r="C265" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D265" s="2"/>
       <c r="E265" s="2"/>
@@ -10820,7 +10820,7 @@
     </row>
     <row r="266" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A266" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B266" s="4"/>
       <c r="C266" s="4"/>
@@ -10849,7 +10849,7 @@
     </row>
     <row r="267" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A267" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B267" s="4"/>
       <c r="C267" s="4"/>
@@ -10878,7 +10878,7 @@
     </row>
     <row r="268" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A268" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B268" s="4"/>
       <c r="C268" s="4"/>
@@ -10907,7 +10907,7 @@
     </row>
     <row r="269" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A269" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B269" s="4"/>
       <c r="C269" s="4"/>
@@ -10936,7 +10936,7 @@
     </row>
     <row r="270" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A270" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B270" s="4"/>
       <c r="C270" s="4"/>
@@ -10965,11 +10965,11 @@
     </row>
     <row r="271" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A271" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B271" s="4"/>
       <c r="C271" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D271" s="2"/>
       <c r="E271" s="2"/>
@@ -10996,11 +10996,11 @@
     </row>
     <row r="272" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A272" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B272" s="4"/>
       <c r="C272" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D272" s="2"/>
       <c r="E272" s="2"/>
@@ -11027,11 +11027,11 @@
     </row>
     <row r="273" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A273" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B273" s="4"/>
       <c r="C273" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D273" s="2"/>
       <c r="E273" s="2"/>
@@ -11058,10 +11058,10 @@
     </row>
     <row r="274" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A274" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="B274" s="4" t="s">
         <v>438</v>
-      </c>
-      <c r="B274" s="4" t="s">
-        <v>439</v>
       </c>
       <c r="C274" s="4"/>
       <c r="D274" s="2"/>
@@ -11089,7 +11089,7 @@
     </row>
     <row r="275" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A275" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B275" s="4"/>
       <c r="C275" s="4"/>
@@ -11118,11 +11118,11 @@
     </row>
     <row r="276" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A276" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B276" s="4"/>
       <c r="C276" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D276" s="2"/>
       <c r="E276" s="2"/>
@@ -11149,7 +11149,7 @@
     </row>
     <row r="277" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A277" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B277" s="4"/>
       <c r="C277" s="4"/>
@@ -11178,11 +11178,11 @@
     </row>
     <row r="278" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A278" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B278" s="4"/>
       <c r="C278" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D278" s="2"/>
       <c r="E278" s="2"/>
@@ -11209,10 +11209,10 @@
     </row>
     <row r="279" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A279" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B279" s="4" t="s">
         <v>446</v>
-      </c>
-      <c r="B279" s="4" t="s">
-        <v>447</v>
       </c>
       <c r="C279" s="4"/>
       <c r="D279" s="2"/>
@@ -11240,7 +11240,7 @@
     </row>
     <row r="280" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A280" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B280" s="4"/>
       <c r="C280" s="4"/>
@@ -11269,11 +11269,11 @@
     </row>
     <row r="281" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A281" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B281" s="4"/>
       <c r="C281" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D281" s="2"/>
       <c r="E281" s="2"/>
@@ -11300,11 +11300,11 @@
     </row>
     <row r="282" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A282" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B282" s="4"/>
       <c r="C282" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D282" s="2"/>
       <c r="E282" s="2"/>
@@ -11331,7 +11331,7 @@
     </row>
     <row r="283" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A283" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B283" s="4"/>
       <c r="C283" s="4"/>
@@ -11360,7 +11360,7 @@
     </row>
     <row r="284" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A284" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B284" s="4"/>
       <c r="C284" s="4"/>
@@ -11389,11 +11389,11 @@
     </row>
     <row r="285" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A285" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B285" s="4"/>
       <c r="C285" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D285" s="2"/>
       <c r="E285" s="2"/>
@@ -11420,11 +11420,11 @@
     </row>
     <row r="286" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A286" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B286" s="4"/>
       <c r="C286" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D286" s="2"/>
       <c r="E286" s="2"/>
@@ -11451,7 +11451,7 @@
     </row>
     <row r="287" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A287" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B287" s="4"/>
       <c r="C287" s="4"/>
@@ -11480,10 +11480,10 @@
     </row>
     <row r="288" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A288" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="B288" s="4" t="s">
         <v>460</v>
-      </c>
-      <c r="B288" s="4" t="s">
-        <v>461</v>
       </c>
       <c r="C288" s="4"/>
       <c r="D288" s="2"/>
@@ -11511,11 +11511,11 @@
     </row>
     <row r="289" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A289" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B289" s="4"/>
       <c r="C289" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D289" s="2"/>
       <c r="E289" s="2"/>
@@ -11542,11 +11542,11 @@
     </row>
     <row r="290" spans="1:25" ht="130" x14ac:dyDescent="0.15">
       <c r="A290" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B290" s="4"/>
       <c r="C290" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D290" s="2"/>
       <c r="E290" s="2"/>
@@ -11573,11 +11573,11 @@
     </row>
     <row r="291" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A291" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B291" s="4"/>
       <c r="C291" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D291" s="2"/>
       <c r="E291" s="2"/>
@@ -11604,7 +11604,7 @@
     </row>
     <row r="292" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A292" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B292" s="4"/>
       <c r="C292" s="4"/>
@@ -11633,7 +11633,7 @@
     </row>
     <row r="293" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A293" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B293" s="4"/>
       <c r="C293" s="4"/>
@@ -11662,7 +11662,7 @@
     </row>
     <row r="294" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A294" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B294" s="4"/>
       <c r="C294" s="4"/>
@@ -11691,7 +11691,7 @@
     </row>
     <row r="295" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A295" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B295" s="4"/>
       <c r="C295" s="4"/>
@@ -11720,7 +11720,7 @@
     </row>
     <row r="296" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A296" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B296" s="4"/>
       <c r="C296" s="4"/>
@@ -11749,7 +11749,7 @@
     </row>
     <row r="297" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A297" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B297" s="4"/>
       <c r="C297" s="4"/>
@@ -11778,11 +11778,11 @@
     </row>
     <row r="298" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A298" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B298" s="4"/>
       <c r="C298" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D298" s="2"/>
       <c r="E298" s="2"/>
@@ -11809,7 +11809,7 @@
     </row>
     <row r="299" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A299" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B299" s="4"/>
       <c r="C299" s="4"/>
@@ -11838,7 +11838,7 @@
     </row>
     <row r="300" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A300" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B300" s="4"/>
       <c r="C300" s="4"/>
@@ -11867,7 +11867,7 @@
     </row>
     <row r="301" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A301" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B301" s="4"/>
       <c r="C301" s="4"/>
@@ -11896,7 +11896,7 @@
     </row>
     <row r="302" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A302" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B302" s="4"/>
       <c r="C302" s="4"/>
@@ -11925,7 +11925,7 @@
     </row>
     <row r="303" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A303" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B303" s="4"/>
       <c r="C303" s="4"/>
@@ -11954,10 +11954,10 @@
     </row>
     <row r="304" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A304" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="B304" s="4" t="s">
         <v>481</v>
-      </c>
-      <c r="B304" s="4" t="s">
-        <v>482</v>
       </c>
       <c r="C304" s="4"/>
       <c r="D304" s="2"/>
@@ -11985,7 +11985,7 @@
     </row>
     <row r="305" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A305" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B305" s="4"/>
       <c r="C305" s="4"/>
@@ -12014,11 +12014,11 @@
     </row>
     <row r="306" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A306" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B306" s="4"/>
       <c r="C306" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D306" s="2"/>
       <c r="E306" s="2"/>
@@ -12045,11 +12045,11 @@
     </row>
     <row r="307" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A307" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B307" s="4"/>
       <c r="C307" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D307" s="2"/>
       <c r="E307" s="2"/>
@@ -12076,11 +12076,11 @@
     </row>
     <row r="308" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A308" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B308" s="4"/>
       <c r="C308" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D308" s="2"/>
       <c r="E308" s="2"/>
@@ -12107,7 +12107,7 @@
     </row>
     <row r="309" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A309" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B309" s="4"/>
       <c r="C309" s="4"/>
@@ -12136,11 +12136,11 @@
     </row>
     <row r="310" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A310" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B310" s="4"/>
       <c r="C310" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D310" s="2"/>
       <c r="E310" s="2"/>
@@ -12167,7 +12167,7 @@
     </row>
     <row r="311" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A311" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B311" s="4"/>
       <c r="C311" s="4"/>
@@ -12196,11 +12196,11 @@
     </row>
     <row r="312" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A312" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B312" s="4"/>
       <c r="C312" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D312" s="2"/>
       <c r="E312" s="2"/>
@@ -12227,7 +12227,7 @@
     </row>
     <row r="313" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A313" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B313" s="4"/>
       <c r="C313" s="4"/>
@@ -12256,7 +12256,7 @@
     </row>
     <row r="314" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A314" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B314" s="4"/>
       <c r="C314" s="4"/>
@@ -12285,11 +12285,11 @@
     </row>
     <row r="315" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A315" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B315" s="4"/>
       <c r="C315" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D315" s="2"/>
       <c r="E315" s="2"/>
@@ -12316,7 +12316,7 @@
     </row>
     <row r="316" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A316" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B316" s="4"/>
       <c r="C316" s="4"/>
@@ -12345,11 +12345,11 @@
     </row>
     <row r="317" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A317" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B317" s="4"/>
       <c r="C317" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D317" s="2"/>
       <c r="E317" s="2"/>
@@ -12376,11 +12376,11 @@
     </row>
     <row r="318" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A318" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B318" s="4"/>
       <c r="C318" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D318" s="2"/>
       <c r="E318" s="2"/>
@@ -12407,7 +12407,7 @@
     </row>
     <row r="319" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A319" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B319" s="4"/>
       <c r="C319" s="4"/>
@@ -12436,11 +12436,11 @@
     </row>
     <row r="320" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A320" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B320" s="4"/>
       <c r="C320" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D320" s="2"/>
       <c r="E320" s="2"/>
@@ -12467,7 +12467,7 @@
     </row>
     <row r="321" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A321" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B321" s="4"/>
       <c r="C321" s="4"/>
@@ -12496,7 +12496,7 @@
     </row>
     <row r="322" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A322" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B322" s="4"/>
       <c r="C322" s="4"/>
@@ -12525,11 +12525,11 @@
     </row>
     <row r="323" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A323" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B323" s="4"/>
       <c r="C323" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D323" s="2"/>
       <c r="E323" s="2"/>
@@ -12556,7 +12556,7 @@
     </row>
     <row r="324" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A324" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B324" s="4"/>
       <c r="C324" s="4"/>
@@ -12585,7 +12585,7 @@
     </row>
     <row r="325" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A325" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B325" s="4"/>
       <c r="C325" s="4"/>
@@ -12614,11 +12614,11 @@
     </row>
     <row r="326" spans="1:25" ht="143" x14ac:dyDescent="0.15">
       <c r="A326" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B326" s="4"/>
       <c r="C326" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D326" s="2"/>
       <c r="E326" s="2"/>
@@ -12645,11 +12645,11 @@
     </row>
     <row r="327" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A327" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B327" s="4"/>
       <c r="C327" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D327" s="2"/>
       <c r="E327" s="2"/>
@@ -12676,7 +12676,7 @@
     </row>
     <row r="328" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A328" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B328" s="4"/>
       <c r="C328" s="4"/>
@@ -12705,11 +12705,11 @@
     </row>
     <row r="329" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A329" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B329" s="4"/>
       <c r="C329" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D329" s="2"/>
       <c r="E329" s="2"/>
@@ -12736,7 +12736,7 @@
     </row>
     <row r="330" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A330" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B330" s="4"/>
       <c r="D330" s="2"/>
@@ -12764,11 +12764,11 @@
     </row>
     <row r="331" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A331" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B331" s="4"/>
       <c r="C331" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D331" s="2"/>
       <c r="E331" s="2"/>
@@ -12795,11 +12795,11 @@
     </row>
     <row r="332" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A332" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B332" s="4"/>
       <c r="C332" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D332" s="2"/>
       <c r="E332" s="2"/>
@@ -12826,7 +12826,7 @@
     </row>
     <row r="333" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A333" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B333" s="4"/>
       <c r="C333" s="4"/>
@@ -12855,7 +12855,7 @@
     </row>
     <row r="334" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A334" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B334" s="4"/>
       <c r="C334" s="4"/>
@@ -12884,11 +12884,11 @@
     </row>
     <row r="335" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A335" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B335" s="4"/>
       <c r="C335" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D335" s="2"/>
       <c r="E335" s="2"/>
@@ -12915,7 +12915,7 @@
     </row>
     <row r="336" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A336" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B336" s="4"/>
       <c r="C336" s="4"/>
@@ -12944,7 +12944,7 @@
     </row>
     <row r="337" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A337" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B337" s="4"/>
       <c r="C337" s="4"/>
@@ -12973,11 +12973,11 @@
     </row>
     <row r="338" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A338" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B338" s="4"/>
       <c r="C338" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D338" s="2"/>
       <c r="E338" s="2"/>
@@ -13004,7 +13004,7 @@
     </row>
     <row r="339" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A339" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B339" s="4"/>
       <c r="C339" s="4"/>
@@ -13033,11 +13033,11 @@
     </row>
     <row r="340" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A340" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B340" s="4"/>
       <c r="C340" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D340" s="2"/>
       <c r="E340" s="2"/>
@@ -13064,7 +13064,7 @@
     </row>
     <row r="341" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A341" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B341" s="4"/>
       <c r="C341" s="4"/>
@@ -13093,10 +13093,10 @@
     </row>
     <row r="342" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A342" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="B342" s="4" t="s">
         <v>538</v>
-      </c>
-      <c r="B342" s="4" t="s">
-        <v>539</v>
       </c>
       <c r="C342" s="4"/>
       <c r="D342" s="2"/>
@@ -13124,7 +13124,7 @@
     </row>
     <row r="343" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A343" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B343" s="4"/>
       <c r="C343" s="4"/>
@@ -13153,7 +13153,7 @@
     </row>
     <row r="344" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A344" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B344" s="4"/>
       <c r="C344" s="4"/>
@@ -13182,7 +13182,7 @@
     </row>
     <row r="345" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A345" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B345" s="4"/>
       <c r="C345" s="4"/>
@@ -13211,11 +13211,11 @@
     </row>
     <row r="346" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A346" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B346" s="4"/>
       <c r="C346" s="4" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D346" s="2"/>
       <c r="E346" s="2"/>
@@ -13242,11 +13242,11 @@
     </row>
     <row r="347" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A347" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B347" s="4"/>
       <c r="C347" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D347" s="2"/>
       <c r="E347" s="2"/>
@@ -13273,10 +13273,10 @@
     </row>
     <row r="348" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A348" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="B348" s="4" t="s">
         <v>547</v>
-      </c>
-      <c r="B348" s="4" t="s">
-        <v>548</v>
       </c>
       <c r="C348" s="4"/>
       <c r="D348" s="2"/>
@@ -13304,11 +13304,11 @@
     </row>
     <row r="349" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A349" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B349" s="4"/>
       <c r="C349" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D349" s="2"/>
       <c r="E349" s="2"/>
@@ -13335,7 +13335,7 @@
     </row>
     <row r="350" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A350" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B350" s="4"/>
       <c r="C350" s="4"/>
@@ -13364,11 +13364,11 @@
     </row>
     <row r="351" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A351" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B351" s="4"/>
       <c r="C351" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D351" s="2"/>
       <c r="E351" s="2"/>
@@ -13395,7 +13395,7 @@
     </row>
     <row r="352" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A352" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B352" s="4"/>
       <c r="C352" s="4"/>
@@ -13424,11 +13424,11 @@
     </row>
     <row r="353" spans="1:25" ht="143" x14ac:dyDescent="0.15">
       <c r="A353" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B353" s="4"/>
       <c r="C353" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D353" s="2"/>
       <c r="E353" s="2"/>
@@ -13455,10 +13455,10 @@
     </row>
     <row r="354" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A354" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B354" s="4" t="s">
         <v>557</v>
-      </c>
-      <c r="B354" s="4" t="s">
-        <v>558</v>
       </c>
       <c r="C354" s="4"/>
       <c r="D354" s="2"/>
@@ -13486,11 +13486,11 @@
     </row>
     <row r="355" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A355" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B355" s="4"/>
       <c r="C355" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D355" s="2"/>
       <c r="E355" s="2"/>
@@ -13517,11 +13517,11 @@
     </row>
     <row r="356" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A356" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B356" s="4"/>
       <c r="C356" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D356" s="2"/>
       <c r="E356" s="2"/>
@@ -13548,7 +13548,7 @@
     </row>
     <row r="357" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A357" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B357" s="4"/>
       <c r="C357" s="4"/>
@@ -13577,10 +13577,10 @@
     </row>
     <row r="358" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A358" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B358" s="4" t="s">
         <v>562</v>
-      </c>
-      <c r="B358" s="4" t="s">
-        <v>563</v>
       </c>
       <c r="C358" s="4"/>
       <c r="D358" s="2"/>
@@ -13608,7 +13608,7 @@
     </row>
     <row r="359" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A359" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B359" s="4"/>
       <c r="C359" s="4"/>
@@ -13637,7 +13637,7 @@
     </row>
     <row r="360" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A360" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B360" s="4"/>
       <c r="C360" s="4"/>
@@ -13666,7 +13666,7 @@
     </row>
     <row r="361" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A361" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B361" s="4"/>
       <c r="C361" s="4"/>
@@ -13695,10 +13695,10 @@
     </row>
     <row r="362" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A362" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="B362" s="4" t="s">
         <v>567</v>
-      </c>
-      <c r="B362" s="4" t="s">
-        <v>568</v>
       </c>
       <c r="C362" s="4"/>
       <c r="D362" s="2"/>
@@ -13726,10 +13726,10 @@
     </row>
     <row r="363" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A363" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="B363" s="4" t="s">
         <v>569</v>
-      </c>
-      <c r="B363" s="4" t="s">
-        <v>570</v>
       </c>
       <c r="C363" s="4"/>
       <c r="D363" s="2"/>
@@ -13757,10 +13757,10 @@
     </row>
     <row r="364" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A364" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="B364" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="B364" s="4" t="s">
-        <v>572</v>
       </c>
       <c r="C364" s="4"/>
       <c r="D364" s="2"/>
@@ -13788,11 +13788,11 @@
     </row>
     <row r="365" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A365" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B365" s="4"/>
       <c r="C365" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D365" s="2"/>
       <c r="E365" s="2"/>
@@ -13819,7 +13819,7 @@
     </row>
     <row r="366" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A366" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B366" s="4"/>
       <c r="C366" s="4"/>
@@ -13848,7 +13848,7 @@
     </row>
     <row r="367" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A367" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B367" s="4"/>
       <c r="C367" s="4"/>
@@ -13877,7 +13877,7 @@
     </row>
     <row r="368" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A368" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B368" s="4"/>
       <c r="C368" s="4"/>
@@ -13906,7 +13906,7 @@
     </row>
     <row r="369" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A369" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B369" s="4"/>
       <c r="C369" s="4"/>
@@ -13935,11 +13935,11 @@
     </row>
     <row r="370" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A370" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B370" s="4"/>
       <c r="C370" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D370" s="2"/>
       <c r="E370" s="2"/>
@@ -13966,7 +13966,7 @@
     </row>
     <row r="371" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A371" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B371" s="4"/>
       <c r="C371" s="4"/>
@@ -13995,10 +13995,10 @@
     </row>
     <row r="372" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A372" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="B372" s="4" t="s">
         <v>582</v>
-      </c>
-      <c r="B372" s="4" t="s">
-        <v>583</v>
       </c>
       <c r="C372" s="4"/>
       <c r="D372" s="2"/>
@@ -14026,7 +14026,7 @@
     </row>
     <row r="373" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A373" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B373" s="4"/>
       <c r="C373" s="4"/>
@@ -14055,7 +14055,7 @@
     </row>
     <row r="374" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A374" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B374" s="4"/>
       <c r="C374" s="4"/>
@@ -14084,7 +14084,7 @@
     </row>
     <row r="375" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A375" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B375" s="4"/>
       <c r="C375" s="4"/>
@@ -14113,10 +14113,10 @@
     </row>
     <row r="376" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A376" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="B376" s="4" t="s">
         <v>587</v>
-      </c>
-      <c r="B376" s="4" t="s">
-        <v>588</v>
       </c>
       <c r="C376" s="4"/>
       <c r="D376" s="2"/>
@@ -14144,10 +14144,10 @@
     </row>
     <row r="377" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A377" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="B377" s="4" t="s">
         <v>589</v>
-      </c>
-      <c r="B377" s="4" t="s">
-        <v>590</v>
       </c>
       <c r="C377" s="4"/>
       <c r="D377" s="2"/>
@@ -14175,10 +14175,10 @@
     </row>
     <row r="378" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A378" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="B378" s="4" t="s">
         <v>591</v>
-      </c>
-      <c r="B378" s="4" t="s">
-        <v>592</v>
       </c>
       <c r="C378" s="4"/>
       <c r="D378" s="2"/>
@@ -14206,11 +14206,11 @@
     </row>
     <row r="379" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A379" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B379" s="4"/>
       <c r="C379" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D379" s="2"/>
       <c r="E379" s="2"/>
@@ -14237,13 +14237,13 @@
     </row>
     <row r="380" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A380" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="B380" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="B380" s="4" t="s">
+      <c r="C380" s="4" t="s">
         <v>596</v>
-      </c>
-      <c r="C380" s="4" t="s">
-        <v>597</v>
       </c>
       <c r="D380" s="2"/>
       <c r="E380" s="2"/>
@@ -14270,11 +14270,11 @@
     </row>
     <row r="381" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A381" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B381" s="4"/>
       <c r="C381" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D381" s="2"/>
       <c r="E381" s="2"/>
@@ -14301,7 +14301,7 @@
     </row>
     <row r="382" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A382" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B382" s="4"/>
       <c r="C382" s="4"/>
@@ -14330,11 +14330,11 @@
     </row>
     <row r="383" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A383" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B383" s="4"/>
       <c r="C383" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D383" s="2"/>
       <c r="E383" s="2"/>
@@ -14361,11 +14361,11 @@
     </row>
     <row r="384" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A384" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B384" s="4"/>
       <c r="C384" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D384" s="2"/>
       <c r="E384" s="2"/>
@@ -14392,10 +14392,10 @@
     </row>
     <row r="385" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A385" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="B385" s="4" t="s">
         <v>605</v>
-      </c>
-      <c r="B385" s="4" t="s">
-        <v>606</v>
       </c>
       <c r="C385" s="4"/>
       <c r="D385" s="2"/>
@@ -14423,11 +14423,11 @@
     </row>
     <row r="386" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A386" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B386" s="4"/>
       <c r="C386" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D386" s="2"/>
       <c r="E386" s="2"/>
@@ -14454,11 +14454,11 @@
     </row>
     <row r="387" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A387" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B387" s="4"/>
       <c r="C387" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D387" s="2"/>
       <c r="E387" s="2"/>
@@ -14485,7 +14485,7 @@
     </row>
     <row r="388" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A388" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B388" s="4"/>
       <c r="C388" s="4"/>
@@ -14514,7 +14514,7 @@
     </row>
     <row r="389" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A389" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B389" s="4"/>
       <c r="C389" s="4"/>
@@ -14543,7 +14543,7 @@
     </row>
     <row r="390" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A390" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B390" s="4"/>
       <c r="C390" s="4"/>
@@ -14572,10 +14572,10 @@
     </row>
     <row r="391" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A391" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="B391" s="4" t="s">
         <v>614</v>
-      </c>
-      <c r="B391" s="4" t="s">
-        <v>615</v>
       </c>
       <c r="C391" s="4"/>
       <c r="D391" s="2"/>
@@ -14603,11 +14603,11 @@
     </row>
     <row r="392" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A392" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B392" s="4"/>
       <c r="C392" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D392" s="2"/>
       <c r="E392" s="2"/>
@@ -14634,11 +14634,11 @@
     </row>
     <row r="393" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A393" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B393" s="4"/>
       <c r="C393" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D393" s="2"/>
       <c r="E393" s="2"/>
@@ -14665,10 +14665,10 @@
     </row>
     <row r="394" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A394" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="B394" s="4" t="s">
         <v>620</v>
-      </c>
-      <c r="B394" s="4" t="s">
-        <v>621</v>
       </c>
       <c r="C394" s="4"/>
       <c r="D394" s="2"/>
@@ -14696,11 +14696,11 @@
     </row>
     <row r="395" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A395" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B395" s="4"/>
       <c r="C395" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D395" s="2"/>
       <c r="E395" s="2"/>
@@ -14727,11 +14727,11 @@
     </row>
     <row r="396" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A396" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B396" s="4"/>
       <c r="C396" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D396" s="2"/>
       <c r="E396" s="2"/>
@@ -14758,11 +14758,11 @@
     </row>
     <row r="397" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A397" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B397" s="4"/>
       <c r="C397" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D397" s="2"/>
       <c r="E397" s="2"/>
@@ -14789,10 +14789,10 @@
     </row>
     <row r="398" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A398" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="B398" s="4" t="s">
         <v>628</v>
-      </c>
-      <c r="B398" s="4" t="s">
-        <v>629</v>
       </c>
       <c r="C398" s="4"/>
       <c r="D398" s="2"/>
@@ -14820,7 +14820,7 @@
     </row>
     <row r="399" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A399" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B399" s="4"/>
       <c r="C399" s="4"/>
@@ -14849,11 +14849,11 @@
     </row>
     <row r="400" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A400" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B400" s="4"/>
       <c r="C400" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D400" s="2"/>
       <c r="E400" s="2"/>
@@ -14880,10 +14880,10 @@
     </row>
     <row r="401" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A401" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="B401" s="4" t="s">
         <v>633</v>
-      </c>
-      <c r="B401" s="4" t="s">
-        <v>634</v>
       </c>
       <c r="C401" s="4"/>
       <c r="D401" s="2"/>
@@ -14911,11 +14911,11 @@
     </row>
     <row r="402" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A402" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B402" s="4"/>
       <c r="C402" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D402" s="2"/>
       <c r="E402" s="2"/>
@@ -14942,7 +14942,7 @@
     </row>
     <row r="403" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A403" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B403" s="4"/>
       <c r="C403" s="4"/>
@@ -14971,7 +14971,7 @@
     </row>
     <row r="404" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A404" s="4" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B404" s="4"/>
       <c r="C404" s="4"/>
@@ -15000,11 +15000,11 @@
     </row>
     <row r="405" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A405" s="4" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B405" s="4"/>
       <c r="C405" s="4" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D405" s="2"/>
       <c r="E405" s="2"/>
@@ -15031,7 +15031,7 @@
     </row>
     <row r="406" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A406" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B406" s="4"/>
       <c r="C406" s="4"/>
@@ -15060,11 +15060,11 @@
     </row>
     <row r="407" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A407" s="4" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B407" s="4"/>
       <c r="C407" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D407" s="2"/>
       <c r="E407" s="2"/>
@@ -15091,7 +15091,7 @@
     </row>
     <row r="408" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A408" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B408" s="4"/>
       <c r="C408" s="4"/>
@@ -15120,7 +15120,7 @@
     </row>
     <row r="409" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A409" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B409" s="4"/>
       <c r="C409" s="4"/>
@@ -15149,7 +15149,7 @@
     </row>
     <row r="410" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A410" s="4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B410" s="4"/>
       <c r="C410" s="4"/>
@@ -15178,7 +15178,7 @@
     </row>
     <row r="411" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A411" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B411" s="4"/>
       <c r="C411" s="4"/>
@@ -15207,10 +15207,10 @@
     </row>
     <row r="412" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A412" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="B412" s="4" t="s">
         <v>648</v>
-      </c>
-      <c r="B412" s="4" t="s">
-        <v>649</v>
       </c>
       <c r="C412" s="4"/>
       <c r="D412" s="2"/>
@@ -15238,7 +15238,7 @@
     </row>
     <row r="413" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A413" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B413" s="4"/>
       <c r="C413" s="4"/>
@@ -15267,7 +15267,7 @@
     </row>
     <row r="414" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A414" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B414" s="4"/>
       <c r="C414" s="4"/>
@@ -15296,7 +15296,7 @@
     </row>
     <row r="415" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A415" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B415" s="4"/>
       <c r="C415" s="4"/>
@@ -15325,7 +15325,7 @@
     </row>
     <row r="416" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A416" s="4" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B416" s="4"/>
       <c r="C416" s="4"/>
@@ -15354,7 +15354,7 @@
     </row>
     <row r="417" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A417" s="4" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B417" s="4"/>
       <c r="C417" s="4"/>
@@ -15383,7 +15383,7 @@
     </row>
     <row r="418" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A418" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B418" s="4"/>
       <c r="C418" s="2"/>
@@ -15412,7 +15412,7 @@
     </row>
     <row r="419" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A419" s="4" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B419" s="4"/>
       <c r="C419" s="2"/>
@@ -15441,7 +15441,7 @@
     </row>
     <row r="420" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A420" s="4" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B420" s="4"/>
       <c r="C420" s="2"/>
@@ -15470,10 +15470,10 @@
     </row>
     <row r="421" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A421" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="B421" s="4" t="s">
         <v>658</v>
-      </c>
-      <c r="B421" s="4" t="s">
-        <v>659</v>
       </c>
       <c r="C421" s="2"/>
       <c r="D421" s="2"/>

</xml_diff>

<commit_message>
Fix typo weird spacing wikipathways names x2
</commit_message>
<xml_diff>
--- a/mappings/wikipathways_reactome.xlsx
+++ b/mappings/wikipathways_reactome.xlsx
@@ -2372,9 +2372,6 @@
     <t xml:space="preserve">p38 MAPK Signaling Pathway equivalentTo p38MAPK events </t>
   </si>
   <si>
-    <t>Canonical and  Non-canonical Notch signaling</t>
-  </si>
-  <si>
     <t xml:space="preserve">Canonical  and Non-canonical Notch signaling equivalentTo Signaling by NOTCH </t>
   </si>
   <si>
@@ -2416,6 +2413,9 @@
   </si>
   <si>
     <t>Farnesoid X Receptor  Pathway</t>
+  </si>
+  <si>
+    <t>Canonical  and Non-canonical Notch signaling</t>
   </si>
 </sst>
 </file>
@@ -2782,8 +2782,8 @@
   </sheetPr>
   <dimension ref="A1:Y999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="60" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="60" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2803,7 +2803,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -3010,7 +3010,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -4311,13 +4311,13 @@
     </row>
     <row r="51" spans="1:25" ht="409" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>660</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>661</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="122" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -7038,7 +7038,7 @@
         <v>223</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C141" s="4"/>
       <c r="D141" s="2"/>
@@ -8211,7 +8211,7 @@
         <v>282</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C180" s="4"/>
       <c r="D180" s="2"/>
@@ -13517,11 +13517,11 @@
     </row>
     <row r="356" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A356" s="4" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B356" s="4"/>
       <c r="C356" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D356" s="2"/>
       <c r="E356" s="2"/>

</xml_diff>

<commit_message>
Wikipathways beta encoding in one pathway
</commit_message>
<xml_diff>
--- a/mappings/wikipathways_reactome.xlsx
+++ b/mappings/wikipathways_reactome.xlsx
@@ -963,9 +963,6 @@
 Gut-Liver Indole Metabolism* isPartOf Metabolism</t>
   </si>
   <si>
-    <t>H19 action Rb-E2F1 signaling and CDK-��-catenin activity</t>
-  </si>
-  <si>
     <t>HIF1A and PPARG regulation of glycolysis</t>
   </si>
   <si>
@@ -2416,6 +2413,9 @@
   </si>
   <si>
     <t>Canonical  and Non-canonical Notch signaling</t>
+  </si>
+  <si>
+    <t>H19 action Rb-E2F1 signaling and CDK-β-catenin activity</t>
   </si>
 </sst>
 </file>
@@ -2782,8 +2782,8 @@
   </sheetPr>
   <dimension ref="A1:Y999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="60" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="60" workbookViewId="0">
+      <selection activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2803,7 +2803,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -3010,7 +3010,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -4311,13 +4311,13 @@
     </row>
     <row r="51" spans="1:25" ht="409" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>659</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>660</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="122" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -7038,7 +7038,7 @@
         <v>223</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C141" s="4"/>
       <c r="D141" s="2"/>
@@ -7585,7 +7585,7 @@
     </row>
     <row r="159" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="4" t="s">
-        <v>254</v>
+        <v>668</v>
       </c>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
@@ -7614,11 +7614,11 @@
     </row>
     <row r="160" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A160" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B160" s="4"/>
       <c r="C160" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
@@ -7645,7 +7645,7 @@
     </row>
     <row r="161" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A161" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
@@ -7674,10 +7674,10 @@
     </row>
     <row r="162" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B162" s="4" t="s">
         <v>258</v>
-      </c>
-      <c r="B162" s="4" t="s">
-        <v>259</v>
       </c>
       <c r="C162" s="4"/>
       <c r="D162" s="2"/>
@@ -7705,7 +7705,7 @@
     </row>
     <row r="163" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
@@ -7734,7 +7734,7 @@
     </row>
     <row r="164" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A164" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
@@ -7763,10 +7763,10 @@
     </row>
     <row r="165" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B165" s="4" t="s">
         <v>262</v>
-      </c>
-      <c r="B165" s="4" t="s">
-        <v>263</v>
       </c>
       <c r="C165" s="4"/>
       <c r="D165" s="2"/>
@@ -7794,7 +7794,7 @@
     </row>
     <row r="166" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A166" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
@@ -7823,7 +7823,7 @@
     </row>
     <row r="167" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A167" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
@@ -7852,11 +7852,11 @@
     </row>
     <row r="168" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B168" s="4"/>
       <c r="C168" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
@@ -7883,7 +7883,7 @@
     </row>
     <row r="169" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A169" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
@@ -7912,11 +7912,11 @@
     </row>
     <row r="170" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A170" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B170" s="4"/>
       <c r="C170" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
@@ -7943,10 +7943,10 @@
     </row>
     <row r="171" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B171" s="4" t="s">
         <v>271</v>
-      </c>
-      <c r="B171" s="4" t="s">
-        <v>272</v>
       </c>
       <c r="C171" s="4"/>
       <c r="D171" s="2"/>
@@ -7974,7 +7974,7 @@
     </row>
     <row r="172" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A172" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
@@ -8003,7 +8003,7 @@
     </row>
     <row r="173" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A173" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
@@ -8032,7 +8032,7 @@
     </row>
     <row r="174" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A174" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
@@ -8061,7 +8061,7 @@
     </row>
     <row r="175" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A175" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
@@ -8090,7 +8090,7 @@
     </row>
     <row r="176" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A176" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
@@ -8119,7 +8119,7 @@
     </row>
     <row r="177" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A177" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
@@ -8148,7 +8148,7 @@
     </row>
     <row r="178" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A178" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
@@ -8177,10 +8177,10 @@
     </row>
     <row r="179" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A179" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B179" s="4" t="s">
         <v>280</v>
-      </c>
-      <c r="B179" s="4" t="s">
-        <v>281</v>
       </c>
       <c r="C179" s="4"/>
       <c r="D179" s="2"/>
@@ -8208,10 +8208,10 @@
     </row>
     <row r="180" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A180" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C180" s="4"/>
       <c r="D180" s="2"/>
@@ -8239,11 +8239,11 @@
     </row>
     <row r="181" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A181" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B181" s="4"/>
       <c r="C181" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
@@ -8270,11 +8270,11 @@
     </row>
     <row r="182" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A182" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B182" s="4"/>
       <c r="C182" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
@@ -8301,11 +8301,11 @@
     </row>
     <row r="183" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A183" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B183" s="4"/>
       <c r="C183" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
@@ -8332,10 +8332,10 @@
     </row>
     <row r="184" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A184" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B184" s="4" t="s">
         <v>289</v>
-      </c>
-      <c r="B184" s="4" t="s">
-        <v>290</v>
       </c>
       <c r="C184" s="4"/>
       <c r="D184" s="2"/>
@@ -8363,10 +8363,10 @@
     </row>
     <row r="185" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A185" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B185" s="4" t="s">
         <v>291</v>
-      </c>
-      <c r="B185" s="4" t="s">
-        <v>292</v>
       </c>
       <c r="C185" s="4"/>
       <c r="D185" s="2"/>
@@ -8394,10 +8394,10 @@
     </row>
     <row r="186" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B186" s="4" t="s">
         <v>293</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>294</v>
       </c>
       <c r="C186" s="4"/>
       <c r="D186" s="2"/>
@@ -8425,11 +8425,11 @@
     </row>
     <row r="187" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A187" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B187" s="4"/>
       <c r="C187" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
@@ -8456,10 +8456,10 @@
     </row>
     <row r="188" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A188" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B188" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="B188" s="4" t="s">
-        <v>298</v>
       </c>
       <c r="C188" s="4"/>
       <c r="D188" s="2"/>
@@ -8487,7 +8487,7 @@
     </row>
     <row r="189" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A189" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
@@ -8516,11 +8516,11 @@
     </row>
     <row r="190" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A190" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B190" s="4"/>
       <c r="C190" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
@@ -8547,11 +8547,11 @@
     </row>
     <row r="191" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A191" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B191" s="4"/>
       <c r="C191" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
@@ -8578,7 +8578,7 @@
     </row>
     <row r="192" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A192" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
@@ -8607,7 +8607,7 @@
     </row>
     <row r="193" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A193" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B193" s="4"/>
       <c r="C193" s="4"/>
@@ -8636,11 +8636,11 @@
     </row>
     <row r="194" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A194" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B194" s="4"/>
       <c r="C194" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
@@ -8667,11 +8667,11 @@
     </row>
     <row r="195" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A195" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B195" s="4"/>
       <c r="C195" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
@@ -8698,7 +8698,7 @@
     </row>
     <row r="196" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A196" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B196" s="4"/>
       <c r="C196" s="4"/>
@@ -8727,11 +8727,11 @@
     </row>
     <row r="197" spans="1:25" ht="130" x14ac:dyDescent="0.15">
       <c r="A197" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B197" s="4"/>
       <c r="C197" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
@@ -8758,11 +8758,11 @@
     </row>
     <row r="198" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A198" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B198" s="4"/>
       <c r="C198" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D198" s="2"/>
       <c r="E198" s="2"/>
@@ -8789,7 +8789,7 @@
     </row>
     <row r="199" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A199" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B199" s="4"/>
       <c r="C199" s="4"/>
@@ -8818,11 +8818,11 @@
     </row>
     <row r="200" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A200" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B200" s="4"/>
       <c r="C200" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
@@ -8849,11 +8849,11 @@
     </row>
     <row r="201" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A201" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B201" s="4"/>
       <c r="C201" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
@@ -8880,11 +8880,11 @@
     </row>
     <row r="202" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A202" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B202" s="4"/>
       <c r="C202" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D202" s="2"/>
       <c r="E202" s="2"/>
@@ -8911,7 +8911,7 @@
     </row>
     <row r="203" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A203" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B203" s="4"/>
       <c r="C203" s="4"/>
@@ -8940,11 +8940,11 @@
     </row>
     <row r="204" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A204" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B204" s="4"/>
       <c r="C204" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
@@ -8971,11 +8971,11 @@
     </row>
     <row r="205" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A205" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B205" s="4"/>
       <c r="C205" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D205" s="2"/>
       <c r="E205" s="2"/>
@@ -9002,11 +9002,11 @@
     </row>
     <row r="206" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A206" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B206" s="4"/>
       <c r="C206" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D206" s="2"/>
       <c r="E206" s="2"/>
@@ -9033,11 +9033,11 @@
     </row>
     <row r="207" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A207" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B207" s="4"/>
       <c r="C207" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
@@ -9064,11 +9064,11 @@
     </row>
     <row r="208" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A208" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B208" s="4"/>
       <c r="C208" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
@@ -9095,10 +9095,10 @@
     </row>
     <row r="209" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A209" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B209" s="4" t="s">
         <v>333</v>
-      </c>
-      <c r="B209" s="4" t="s">
-        <v>334</v>
       </c>
       <c r="C209" s="4"/>
       <c r="D209" s="2"/>
@@ -9126,11 +9126,11 @@
     </row>
     <row r="210" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A210" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B210" s="4"/>
       <c r="C210" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D210" s="2"/>
       <c r="E210" s="2"/>
@@ -9157,10 +9157,10 @@
     </row>
     <row r="211" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A211" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B211" s="4" t="s">
         <v>337</v>
-      </c>
-      <c r="B211" s="4" t="s">
-        <v>338</v>
       </c>
       <c r="C211" s="4"/>
       <c r="D211" s="2"/>
@@ -9188,11 +9188,11 @@
     </row>
     <row r="212" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A212" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B212" s="4"/>
       <c r="C212" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D212" s="2"/>
       <c r="E212" s="2"/>
@@ -9219,7 +9219,7 @@
     </row>
     <row r="213" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A213" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B213" s="4"/>
       <c r="C213" s="4"/>
@@ -9248,7 +9248,7 @@
     </row>
     <row r="214" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A214" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B214" s="4"/>
       <c r="C214" s="4"/>
@@ -9277,7 +9277,7 @@
     </row>
     <row r="215" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A215" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B215" s="4"/>
       <c r="C215" s="4"/>
@@ -9306,10 +9306,10 @@
     </row>
     <row r="216" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A216" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B216" s="4" t="s">
         <v>344</v>
-      </c>
-      <c r="B216" s="4" t="s">
-        <v>345</v>
       </c>
       <c r="C216" s="4"/>
       <c r="D216" s="2"/>
@@ -9337,10 +9337,10 @@
     </row>
     <row r="217" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A217" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B217" s="4" t="s">
         <v>346</v>
-      </c>
-      <c r="B217" s="4" t="s">
-        <v>347</v>
       </c>
       <c r="C217" s="4"/>
       <c r="D217" s="2"/>
@@ -9368,7 +9368,7 @@
     </row>
     <row r="218" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A218" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B218" s="4"/>
       <c r="C218" s="4"/>
@@ -9397,7 +9397,7 @@
     </row>
     <row r="219" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A219" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B219" s="4"/>
       <c r="C219" s="4"/>
@@ -9426,11 +9426,11 @@
     </row>
     <row r="220" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A220" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B220" s="4"/>
       <c r="C220" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
@@ -9457,11 +9457,11 @@
     </row>
     <row r="221" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A221" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B221" s="4"/>
       <c r="C221" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
@@ -9488,7 +9488,7 @@
     </row>
     <row r="222" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A222" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B222" s="4"/>
       <c r="C222" s="4"/>
@@ -9517,7 +9517,7 @@
     </row>
     <row r="223" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A223" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B223" s="4"/>
       <c r="C223" s="4"/>
@@ -9546,11 +9546,11 @@
     </row>
     <row r="224" spans="1:25" ht="130" x14ac:dyDescent="0.15">
       <c r="A224" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B224" s="4"/>
       <c r="C224" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
@@ -9577,11 +9577,11 @@
     </row>
     <row r="225" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A225" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B225" s="4"/>
       <c r="C225" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D225" s="2"/>
       <c r="E225" s="2"/>
@@ -9608,7 +9608,7 @@
     </row>
     <row r="226" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A226" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B226" s="4"/>
       <c r="C226" s="4"/>
@@ -9637,7 +9637,7 @@
     </row>
     <row r="227" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A227" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B227" s="4"/>
       <c r="C227" s="4"/>
@@ -9666,13 +9666,13 @@
     </row>
     <row r="228" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A228" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B228" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="B228" s="4" t="s">
+      <c r="C228" s="4" t="s">
         <v>363</v>
-      </c>
-      <c r="C228" s="4" t="s">
-        <v>364</v>
       </c>
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
@@ -9699,10 +9699,10 @@
     </row>
     <row r="229" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A229" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="B229" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="B229" s="4" t="s">
-        <v>366</v>
       </c>
       <c r="C229" s="4"/>
       <c r="D229" s="2"/>
@@ -9730,7 +9730,7 @@
     </row>
     <row r="230" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A230" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B230" s="4"/>
       <c r="C230" s="4"/>
@@ -9759,11 +9759,11 @@
     </row>
     <row r="231" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A231" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B231" s="4"/>
       <c r="C231" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D231" s="2"/>
       <c r="E231" s="2"/>
@@ -9790,10 +9790,10 @@
     </row>
     <row r="232" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A232" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B232" s="4" t="s">
         <v>370</v>
-      </c>
-      <c r="B232" s="4" t="s">
-        <v>371</v>
       </c>
       <c r="C232" s="4"/>
       <c r="D232" s="2"/>
@@ -9821,11 +9821,11 @@
     </row>
     <row r="233" spans="1:25" ht="221" x14ac:dyDescent="0.15">
       <c r="A233" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B233" s="4"/>
       <c r="C233" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
@@ -9852,11 +9852,11 @@
     </row>
     <row r="234" spans="1:25" ht="273" x14ac:dyDescent="0.15">
       <c r="A234" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B234" s="4"/>
       <c r="C234" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
@@ -9883,11 +9883,11 @@
     </row>
     <row r="235" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A235" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B235" s="4"/>
       <c r="C235" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D235" s="2"/>
       <c r="E235" s="2"/>
@@ -9914,11 +9914,11 @@
     </row>
     <row r="236" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A236" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B236" s="4"/>
       <c r="C236" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D236" s="2"/>
       <c r="E236" s="2"/>
@@ -9945,7 +9945,7 @@
     </row>
     <row r="237" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A237" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B237" s="4"/>
       <c r="C237" s="4"/>
@@ -9974,11 +9974,11 @@
     </row>
     <row r="238" spans="1:25" ht="169" x14ac:dyDescent="0.15">
       <c r="A238" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B238" s="4"/>
       <c r="C238" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
@@ -10005,7 +10005,7 @@
     </row>
     <row r="239" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A239" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B239" s="4"/>
       <c r="C239" s="4"/>
@@ -10034,11 +10034,11 @@
     </row>
     <row r="240" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A240" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B240" s="4"/>
       <c r="C240" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
@@ -10065,11 +10065,11 @@
     </row>
     <row r="241" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A241" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B241" s="4"/>
       <c r="C241" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D241" s="2"/>
       <c r="E241" s="2"/>
@@ -10096,11 +10096,11 @@
     </row>
     <row r="242" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A242" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B242" s="4"/>
       <c r="C242" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D242" s="2"/>
       <c r="E242" s="2"/>
@@ -10127,7 +10127,7 @@
     </row>
     <row r="243" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A243" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B243" s="4"/>
       <c r="C243" s="4"/>
@@ -10156,7 +10156,7 @@
     </row>
     <row r="244" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A244" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B244" s="4"/>
       <c r="C244" s="4"/>
@@ -10185,7 +10185,7 @@
     </row>
     <row r="245" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A245" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B245" s="4"/>
       <c r="C245" s="4"/>
@@ -10214,11 +10214,11 @@
     </row>
     <row r="246" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A246" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B246" s="4"/>
       <c r="C246" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D246" s="2"/>
       <c r="E246" s="2"/>
@@ -10245,7 +10245,7 @@
     </row>
     <row r="247" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A247" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B247" s="4"/>
       <c r="C247" s="4"/>
@@ -10274,11 +10274,11 @@
     </row>
     <row r="248" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A248" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B248" s="4"/>
       <c r="C248" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D248" s="2"/>
       <c r="E248" s="2"/>
@@ -10305,7 +10305,7 @@
     </row>
     <row r="249" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A249" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B249" s="4"/>
       <c r="C249" s="4"/>
@@ -10334,7 +10334,7 @@
     </row>
     <row r="250" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A250" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B250" s="4"/>
       <c r="C250" s="4"/>
@@ -10363,11 +10363,11 @@
     </row>
     <row r="251" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A251" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B251" s="4"/>
       <c r="C251" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D251" s="2"/>
       <c r="E251" s="2"/>
@@ -10394,7 +10394,7 @@
     </row>
     <row r="252" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A252" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B252" s="4"/>
       <c r="C252" s="4"/>
@@ -10423,11 +10423,11 @@
     </row>
     <row r="253" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A253" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B253" s="4"/>
       <c r="C253" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D253" s="2"/>
       <c r="E253" s="2"/>
@@ -10454,11 +10454,11 @@
     </row>
     <row r="254" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A254" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B254" s="4"/>
       <c r="C254" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D254" s="2"/>
       <c r="E254" s="2"/>
@@ -10485,10 +10485,10 @@
     </row>
     <row r="255" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A255" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B255" s="4" t="s">
         <v>407</v>
-      </c>
-      <c r="B255" s="4" t="s">
-        <v>408</v>
       </c>
       <c r="C255" s="4"/>
       <c r="D255" s="2"/>
@@ -10516,10 +10516,10 @@
     </row>
     <row r="256" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A256" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B256" s="4" t="s">
         <v>409</v>
-      </c>
-      <c r="B256" s="4" t="s">
-        <v>410</v>
       </c>
       <c r="C256" s="4"/>
       <c r="D256" s="2"/>
@@ -10547,11 +10547,11 @@
     </row>
     <row r="257" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A257" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B257" s="4"/>
       <c r="C257" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D257" s="2"/>
       <c r="E257" s="2"/>
@@ -10578,11 +10578,11 @@
     </row>
     <row r="258" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A258" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B258" s="4"/>
       <c r="C258" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D258" s="2"/>
       <c r="E258" s="2"/>
@@ -10609,7 +10609,7 @@
     </row>
     <row r="259" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A259" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B259" s="4"/>
       <c r="C259" s="4"/>
@@ -10638,10 +10638,10 @@
     </row>
     <row r="260" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A260" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="B260" s="4" t="s">
         <v>416</v>
-      </c>
-      <c r="B260" s="4" t="s">
-        <v>417</v>
       </c>
       <c r="C260" s="4"/>
       <c r="D260" s="2"/>
@@ -10669,7 +10669,7 @@
     </row>
     <row r="261" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A261" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B261" s="4"/>
       <c r="C261" s="4"/>
@@ -10698,7 +10698,7 @@
     </row>
     <row r="262" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A262" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B262" s="4"/>
       <c r="C262" s="4"/>
@@ -10727,11 +10727,11 @@
     </row>
     <row r="263" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A263" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B263" s="4"/>
       <c r="C263" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D263" s="2"/>
       <c r="E263" s="2"/>
@@ -10758,11 +10758,11 @@
     </row>
     <row r="264" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A264" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B264" s="4"/>
       <c r="C264" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D264" s="2"/>
       <c r="E264" s="2"/>
@@ -10789,11 +10789,11 @@
     </row>
     <row r="265" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A265" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B265" s="4"/>
       <c r="C265" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D265" s="2"/>
       <c r="E265" s="2"/>
@@ -10820,7 +10820,7 @@
     </row>
     <row r="266" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A266" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B266" s="4"/>
       <c r="C266" s="4"/>
@@ -10849,7 +10849,7 @@
     </row>
     <row r="267" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A267" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B267" s="4"/>
       <c r="C267" s="4"/>
@@ -10878,7 +10878,7 @@
     </row>
     <row r="268" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A268" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B268" s="4"/>
       <c r="C268" s="4"/>
@@ -10907,7 +10907,7 @@
     </row>
     <row r="269" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A269" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B269" s="4"/>
       <c r="C269" s="4"/>
@@ -10936,7 +10936,7 @@
     </row>
     <row r="270" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A270" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B270" s="4"/>
       <c r="C270" s="4"/>
@@ -10965,11 +10965,11 @@
     </row>
     <row r="271" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A271" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B271" s="4"/>
       <c r="C271" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D271" s="2"/>
       <c r="E271" s="2"/>
@@ -10996,11 +10996,11 @@
     </row>
     <row r="272" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A272" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B272" s="4"/>
       <c r="C272" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D272" s="2"/>
       <c r="E272" s="2"/>
@@ -11027,11 +11027,11 @@
     </row>
     <row r="273" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A273" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B273" s="4"/>
       <c r="C273" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D273" s="2"/>
       <c r="E273" s="2"/>
@@ -11058,10 +11058,10 @@
     </row>
     <row r="274" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A274" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="B274" s="4" t="s">
         <v>437</v>
-      </c>
-      <c r="B274" s="4" t="s">
-        <v>438</v>
       </c>
       <c r="C274" s="4"/>
       <c r="D274" s="2"/>
@@ -11089,7 +11089,7 @@
     </row>
     <row r="275" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A275" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B275" s="4"/>
       <c r="C275" s="4"/>
@@ -11118,11 +11118,11 @@
     </row>
     <row r="276" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A276" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B276" s="4"/>
       <c r="C276" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D276" s="2"/>
       <c r="E276" s="2"/>
@@ -11149,7 +11149,7 @@
     </row>
     <row r="277" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A277" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B277" s="4"/>
       <c r="C277" s="4"/>
@@ -11178,11 +11178,11 @@
     </row>
     <row r="278" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A278" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B278" s="4"/>
       <c r="C278" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D278" s="2"/>
       <c r="E278" s="2"/>
@@ -11209,10 +11209,10 @@
     </row>
     <row r="279" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A279" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="B279" s="4" t="s">
         <v>445</v>
-      </c>
-      <c r="B279" s="4" t="s">
-        <v>446</v>
       </c>
       <c r="C279" s="4"/>
       <c r="D279" s="2"/>
@@ -11240,7 +11240,7 @@
     </row>
     <row r="280" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A280" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B280" s="4"/>
       <c r="C280" s="4"/>
@@ -11269,11 +11269,11 @@
     </row>
     <row r="281" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A281" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B281" s="4"/>
       <c r="C281" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D281" s="2"/>
       <c r="E281" s="2"/>
@@ -11300,11 +11300,11 @@
     </row>
     <row r="282" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A282" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B282" s="4"/>
       <c r="C282" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D282" s="2"/>
       <c r="E282" s="2"/>
@@ -11331,7 +11331,7 @@
     </row>
     <row r="283" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A283" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B283" s="4"/>
       <c r="C283" s="4"/>
@@ -11360,7 +11360,7 @@
     </row>
     <row r="284" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A284" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B284" s="4"/>
       <c r="C284" s="4"/>
@@ -11389,11 +11389,11 @@
     </row>
     <row r="285" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A285" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B285" s="4"/>
       <c r="C285" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D285" s="2"/>
       <c r="E285" s="2"/>
@@ -11420,11 +11420,11 @@
     </row>
     <row r="286" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A286" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B286" s="4"/>
       <c r="C286" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D286" s="2"/>
       <c r="E286" s="2"/>
@@ -11451,7 +11451,7 @@
     </row>
     <row r="287" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A287" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B287" s="4"/>
       <c r="C287" s="4"/>
@@ -11480,10 +11480,10 @@
     </row>
     <row r="288" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A288" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="B288" s="4" t="s">
         <v>459</v>
-      </c>
-      <c r="B288" s="4" t="s">
-        <v>460</v>
       </c>
       <c r="C288" s="4"/>
       <c r="D288" s="2"/>
@@ -11511,11 +11511,11 @@
     </row>
     <row r="289" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A289" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B289" s="4"/>
       <c r="C289" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D289" s="2"/>
       <c r="E289" s="2"/>
@@ -11542,11 +11542,11 @@
     </row>
     <row r="290" spans="1:25" ht="130" x14ac:dyDescent="0.15">
       <c r="A290" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B290" s="4"/>
       <c r="C290" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D290" s="2"/>
       <c r="E290" s="2"/>
@@ -11573,11 +11573,11 @@
     </row>
     <row r="291" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A291" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B291" s="4"/>
       <c r="C291" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D291" s="2"/>
       <c r="E291" s="2"/>
@@ -11604,7 +11604,7 @@
     </row>
     <row r="292" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A292" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B292" s="4"/>
       <c r="C292" s="4"/>
@@ -11633,7 +11633,7 @@
     </row>
     <row r="293" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A293" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B293" s="4"/>
       <c r="C293" s="4"/>
@@ -11662,7 +11662,7 @@
     </row>
     <row r="294" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A294" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B294" s="4"/>
       <c r="C294" s="4"/>
@@ -11691,7 +11691,7 @@
     </row>
     <row r="295" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A295" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B295" s="4"/>
       <c r="C295" s="4"/>
@@ -11720,7 +11720,7 @@
     </row>
     <row r="296" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A296" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B296" s="4"/>
       <c r="C296" s="4"/>
@@ -11749,7 +11749,7 @@
     </row>
     <row r="297" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A297" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B297" s="4"/>
       <c r="C297" s="4"/>
@@ -11778,11 +11778,11 @@
     </row>
     <row r="298" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A298" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B298" s="4"/>
       <c r="C298" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D298" s="2"/>
       <c r="E298" s="2"/>
@@ -11809,7 +11809,7 @@
     </row>
     <row r="299" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A299" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B299" s="4"/>
       <c r="C299" s="4"/>
@@ -11838,7 +11838,7 @@
     </row>
     <row r="300" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A300" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B300" s="4"/>
       <c r="C300" s="4"/>
@@ -11867,7 +11867,7 @@
     </row>
     <row r="301" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A301" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B301" s="4"/>
       <c r="C301" s="4"/>
@@ -11896,7 +11896,7 @@
     </row>
     <row r="302" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A302" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B302" s="4"/>
       <c r="C302" s="4"/>
@@ -11925,7 +11925,7 @@
     </row>
     <row r="303" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A303" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B303" s="4"/>
       <c r="C303" s="4"/>
@@ -11954,10 +11954,10 @@
     </row>
     <row r="304" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A304" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="B304" s="4" t="s">
         <v>480</v>
-      </c>
-      <c r="B304" s="4" t="s">
-        <v>481</v>
       </c>
       <c r="C304" s="4"/>
       <c r="D304" s="2"/>
@@ -11985,7 +11985,7 @@
     </row>
     <row r="305" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A305" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B305" s="4"/>
       <c r="C305" s="4"/>
@@ -12014,11 +12014,11 @@
     </row>
     <row r="306" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A306" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B306" s="4"/>
       <c r="C306" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D306" s="2"/>
       <c r="E306" s="2"/>
@@ -12045,11 +12045,11 @@
     </row>
     <row r="307" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A307" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B307" s="4"/>
       <c r="C307" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D307" s="2"/>
       <c r="E307" s="2"/>
@@ -12076,11 +12076,11 @@
     </row>
     <row r="308" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A308" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B308" s="4"/>
       <c r="C308" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D308" s="2"/>
       <c r="E308" s="2"/>
@@ -12107,7 +12107,7 @@
     </row>
     <row r="309" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A309" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B309" s="4"/>
       <c r="C309" s="4"/>
@@ -12136,11 +12136,11 @@
     </row>
     <row r="310" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A310" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B310" s="4"/>
       <c r="C310" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D310" s="2"/>
       <c r="E310" s="2"/>
@@ -12167,7 +12167,7 @@
     </row>
     <row r="311" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A311" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B311" s="4"/>
       <c r="C311" s="4"/>
@@ -12196,11 +12196,11 @@
     </row>
     <row r="312" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A312" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B312" s="4"/>
       <c r="C312" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D312" s="2"/>
       <c r="E312" s="2"/>
@@ -12227,7 +12227,7 @@
     </row>
     <row r="313" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A313" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B313" s="4"/>
       <c r="C313" s="4"/>
@@ -12256,7 +12256,7 @@
     </row>
     <row r="314" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A314" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B314" s="4"/>
       <c r="C314" s="4"/>
@@ -12285,11 +12285,11 @@
     </row>
     <row r="315" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A315" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B315" s="4"/>
       <c r="C315" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D315" s="2"/>
       <c r="E315" s="2"/>
@@ -12316,7 +12316,7 @@
     </row>
     <row r="316" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A316" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B316" s="4"/>
       <c r="C316" s="4"/>
@@ -12345,11 +12345,11 @@
     </row>
     <row r="317" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A317" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B317" s="4"/>
       <c r="C317" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D317" s="2"/>
       <c r="E317" s="2"/>
@@ -12376,11 +12376,11 @@
     </row>
     <row r="318" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A318" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B318" s="4"/>
       <c r="C318" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D318" s="2"/>
       <c r="E318" s="2"/>
@@ -12407,7 +12407,7 @@
     </row>
     <row r="319" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A319" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B319" s="4"/>
       <c r="C319" s="4"/>
@@ -12436,11 +12436,11 @@
     </row>
     <row r="320" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A320" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B320" s="4"/>
       <c r="C320" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D320" s="2"/>
       <c r="E320" s="2"/>
@@ -12467,7 +12467,7 @@
     </row>
     <row r="321" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A321" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B321" s="4"/>
       <c r="C321" s="4"/>
@@ -12496,7 +12496,7 @@
     </row>
     <row r="322" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A322" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B322" s="4"/>
       <c r="C322" s="4"/>
@@ -12525,11 +12525,11 @@
     </row>
     <row r="323" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A323" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B323" s="4"/>
       <c r="C323" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D323" s="2"/>
       <c r="E323" s="2"/>
@@ -12556,7 +12556,7 @@
     </row>
     <row r="324" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A324" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B324" s="4"/>
       <c r="C324" s="4"/>
@@ -12585,7 +12585,7 @@
     </row>
     <row r="325" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A325" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B325" s="4"/>
       <c r="C325" s="4"/>
@@ -12614,11 +12614,11 @@
     </row>
     <row r="326" spans="1:25" ht="143" x14ac:dyDescent="0.15">
       <c r="A326" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B326" s="4"/>
       <c r="C326" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D326" s="2"/>
       <c r="E326" s="2"/>
@@ -12645,11 +12645,11 @@
     </row>
     <row r="327" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A327" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B327" s="4"/>
       <c r="C327" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D327" s="2"/>
       <c r="E327" s="2"/>
@@ -12676,7 +12676,7 @@
     </row>
     <row r="328" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A328" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B328" s="4"/>
       <c r="C328" s="4"/>
@@ -12705,11 +12705,11 @@
     </row>
     <row r="329" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A329" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B329" s="4"/>
       <c r="C329" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D329" s="2"/>
       <c r="E329" s="2"/>
@@ -12736,7 +12736,7 @@
     </row>
     <row r="330" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A330" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B330" s="4"/>
       <c r="D330" s="2"/>
@@ -12764,11 +12764,11 @@
     </row>
     <row r="331" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A331" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B331" s="4"/>
       <c r="C331" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D331" s="2"/>
       <c r="E331" s="2"/>
@@ -12795,11 +12795,11 @@
     </row>
     <row r="332" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A332" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B332" s="4"/>
       <c r="C332" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D332" s="2"/>
       <c r="E332" s="2"/>
@@ -12826,7 +12826,7 @@
     </row>
     <row r="333" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A333" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B333" s="4"/>
       <c r="C333" s="4"/>
@@ -12855,7 +12855,7 @@
     </row>
     <row r="334" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A334" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B334" s="4"/>
       <c r="C334" s="4"/>
@@ -12884,11 +12884,11 @@
     </row>
     <row r="335" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A335" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B335" s="4"/>
       <c r="C335" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D335" s="2"/>
       <c r="E335" s="2"/>
@@ -12915,7 +12915,7 @@
     </row>
     <row r="336" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A336" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B336" s="4"/>
       <c r="C336" s="4"/>
@@ -12944,7 +12944,7 @@
     </row>
     <row r="337" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A337" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B337" s="4"/>
       <c r="C337" s="4"/>
@@ -12973,11 +12973,11 @@
     </row>
     <row r="338" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A338" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B338" s="4"/>
       <c r="C338" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D338" s="2"/>
       <c r="E338" s="2"/>
@@ -13004,7 +13004,7 @@
     </row>
     <row r="339" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A339" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B339" s="4"/>
       <c r="C339" s="4"/>
@@ -13033,11 +13033,11 @@
     </row>
     <row r="340" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A340" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B340" s="4"/>
       <c r="C340" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D340" s="2"/>
       <c r="E340" s="2"/>
@@ -13064,7 +13064,7 @@
     </row>
     <row r="341" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A341" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B341" s="4"/>
       <c r="C341" s="4"/>
@@ -13093,10 +13093,10 @@
     </row>
     <row r="342" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A342" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="B342" s="4" t="s">
         <v>537</v>
-      </c>
-      <c r="B342" s="4" t="s">
-        <v>538</v>
       </c>
       <c r="C342" s="4"/>
       <c r="D342" s="2"/>
@@ -13124,7 +13124,7 @@
     </row>
     <row r="343" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A343" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B343" s="4"/>
       <c r="C343" s="4"/>
@@ -13153,7 +13153,7 @@
     </row>
     <row r="344" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A344" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B344" s="4"/>
       <c r="C344" s="4"/>
@@ -13182,7 +13182,7 @@
     </row>
     <row r="345" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A345" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B345" s="4"/>
       <c r="C345" s="4"/>
@@ -13211,11 +13211,11 @@
     </row>
     <row r="346" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A346" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B346" s="4"/>
       <c r="C346" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D346" s="2"/>
       <c r="E346" s="2"/>
@@ -13242,11 +13242,11 @@
     </row>
     <row r="347" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A347" s="4" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B347" s="4"/>
       <c r="C347" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D347" s="2"/>
       <c r="E347" s="2"/>
@@ -13273,10 +13273,10 @@
     </row>
     <row r="348" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A348" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="B348" s="4" t="s">
         <v>546</v>
-      </c>
-      <c r="B348" s="4" t="s">
-        <v>547</v>
       </c>
       <c r="C348" s="4"/>
       <c r="D348" s="2"/>
@@ -13304,11 +13304,11 @@
     </row>
     <row r="349" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A349" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B349" s="4"/>
       <c r="C349" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D349" s="2"/>
       <c r="E349" s="2"/>
@@ -13335,7 +13335,7 @@
     </row>
     <row r="350" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A350" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B350" s="4"/>
       <c r="C350" s="4"/>
@@ -13364,11 +13364,11 @@
     </row>
     <row r="351" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A351" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B351" s="4"/>
       <c r="C351" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D351" s="2"/>
       <c r="E351" s="2"/>
@@ -13395,7 +13395,7 @@
     </row>
     <row r="352" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A352" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B352" s="4"/>
       <c r="C352" s="4"/>
@@ -13424,11 +13424,11 @@
     </row>
     <row r="353" spans="1:25" ht="143" x14ac:dyDescent="0.15">
       <c r="A353" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B353" s="4"/>
       <c r="C353" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D353" s="2"/>
       <c r="E353" s="2"/>
@@ -13455,10 +13455,10 @@
     </row>
     <row r="354" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A354" s="4" t="s">
+        <v>555</v>
+      </c>
+      <c r="B354" s="4" t="s">
         <v>556</v>
-      </c>
-      <c r="B354" s="4" t="s">
-        <v>557</v>
       </c>
       <c r="C354" s="4"/>
       <c r="D354" s="2"/>
@@ -13486,11 +13486,11 @@
     </row>
     <row r="355" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A355" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B355" s="4"/>
       <c r="C355" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D355" s="2"/>
       <c r="E355" s="2"/>
@@ -13517,11 +13517,11 @@
     </row>
     <row r="356" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A356" s="4" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B356" s="4"/>
       <c r="C356" s="4" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D356" s="2"/>
       <c r="E356" s="2"/>
@@ -13548,7 +13548,7 @@
     </row>
     <row r="357" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A357" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B357" s="4"/>
       <c r="C357" s="4"/>
@@ -13577,10 +13577,10 @@
     </row>
     <row r="358" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A358" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="B358" s="4" t="s">
         <v>561</v>
-      </c>
-      <c r="B358" s="4" t="s">
-        <v>562</v>
       </c>
       <c r="C358" s="4"/>
       <c r="D358" s="2"/>
@@ -13608,7 +13608,7 @@
     </row>
     <row r="359" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A359" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B359" s="4"/>
       <c r="C359" s="4"/>
@@ -13637,7 +13637,7 @@
     </row>
     <row r="360" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A360" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B360" s="4"/>
       <c r="C360" s="4"/>
@@ -13666,7 +13666,7 @@
     </row>
     <row r="361" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A361" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B361" s="4"/>
       <c r="C361" s="4"/>
@@ -13695,10 +13695,10 @@
     </row>
     <row r="362" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A362" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="B362" s="4" t="s">
         <v>566</v>
-      </c>
-      <c r="B362" s="4" t="s">
-        <v>567</v>
       </c>
       <c r="C362" s="4"/>
       <c r="D362" s="2"/>
@@ -13726,10 +13726,10 @@
     </row>
     <row r="363" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A363" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="B363" s="4" t="s">
         <v>568</v>
-      </c>
-      <c r="B363" s="4" t="s">
-        <v>569</v>
       </c>
       <c r="C363" s="4"/>
       <c r="D363" s="2"/>
@@ -13757,10 +13757,10 @@
     </row>
     <row r="364" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A364" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="B364" s="4" t="s">
         <v>570</v>
-      </c>
-      <c r="B364" s="4" t="s">
-        <v>571</v>
       </c>
       <c r="C364" s="4"/>
       <c r="D364" s="2"/>
@@ -13788,11 +13788,11 @@
     </row>
     <row r="365" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A365" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B365" s="4"/>
       <c r="C365" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D365" s="2"/>
       <c r="E365" s="2"/>
@@ -13819,7 +13819,7 @@
     </row>
     <row r="366" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A366" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B366" s="4"/>
       <c r="C366" s="4"/>
@@ -13848,7 +13848,7 @@
     </row>
     <row r="367" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A367" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B367" s="4"/>
       <c r="C367" s="4"/>
@@ -13877,7 +13877,7 @@
     </row>
     <row r="368" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A368" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B368" s="4"/>
       <c r="C368" s="4"/>
@@ -13906,7 +13906,7 @@
     </row>
     <row r="369" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A369" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B369" s="4"/>
       <c r="C369" s="4"/>
@@ -13935,11 +13935,11 @@
     </row>
     <row r="370" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A370" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B370" s="4"/>
       <c r="C370" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D370" s="2"/>
       <c r="E370" s="2"/>
@@ -13966,7 +13966,7 @@
     </row>
     <row r="371" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A371" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B371" s="4"/>
       <c r="C371" s="4"/>
@@ -13995,10 +13995,10 @@
     </row>
     <row r="372" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A372" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="B372" s="4" t="s">
         <v>581</v>
-      </c>
-      <c r="B372" s="4" t="s">
-        <v>582</v>
       </c>
       <c r="C372" s="4"/>
       <c r="D372" s="2"/>
@@ -14026,7 +14026,7 @@
     </row>
     <row r="373" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A373" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B373" s="4"/>
       <c r="C373" s="4"/>
@@ -14055,7 +14055,7 @@
     </row>
     <row r="374" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A374" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B374" s="4"/>
       <c r="C374" s="4"/>
@@ -14084,7 +14084,7 @@
     </row>
     <row r="375" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A375" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B375" s="4"/>
       <c r="C375" s="4"/>
@@ -14113,10 +14113,10 @@
     </row>
     <row r="376" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A376" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="B376" s="4" t="s">
         <v>586</v>
-      </c>
-      <c r="B376" s="4" t="s">
-        <v>587</v>
       </c>
       <c r="C376" s="4"/>
       <c r="D376" s="2"/>
@@ -14144,10 +14144,10 @@
     </row>
     <row r="377" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A377" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="B377" s="4" t="s">
         <v>588</v>
-      </c>
-      <c r="B377" s="4" t="s">
-        <v>589</v>
       </c>
       <c r="C377" s="4"/>
       <c r="D377" s="2"/>
@@ -14175,10 +14175,10 @@
     </row>
     <row r="378" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A378" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="B378" s="4" t="s">
         <v>590</v>
-      </c>
-      <c r="B378" s="4" t="s">
-        <v>591</v>
       </c>
       <c r="C378" s="4"/>
       <c r="D378" s="2"/>
@@ -14206,11 +14206,11 @@
     </row>
     <row r="379" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A379" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B379" s="4"/>
       <c r="C379" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D379" s="2"/>
       <c r="E379" s="2"/>
@@ -14237,13 +14237,13 @@
     </row>
     <row r="380" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A380" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="B380" s="4" t="s">
         <v>594</v>
       </c>
-      <c r="B380" s="4" t="s">
+      <c r="C380" s="4" t="s">
         <v>595</v>
-      </c>
-      <c r="C380" s="4" t="s">
-        <v>596</v>
       </c>
       <c r="D380" s="2"/>
       <c r="E380" s="2"/>
@@ -14270,11 +14270,11 @@
     </row>
     <row r="381" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A381" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B381" s="4"/>
       <c r="C381" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D381" s="2"/>
       <c r="E381" s="2"/>
@@ -14301,7 +14301,7 @@
     </row>
     <row r="382" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A382" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B382" s="4"/>
       <c r="C382" s="4"/>
@@ -14330,11 +14330,11 @@
     </row>
     <row r="383" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A383" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B383" s="4"/>
       <c r="C383" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D383" s="2"/>
       <c r="E383" s="2"/>
@@ -14361,11 +14361,11 @@
     </row>
     <row r="384" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A384" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B384" s="4"/>
       <c r="C384" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D384" s="2"/>
       <c r="E384" s="2"/>
@@ -14392,10 +14392,10 @@
     </row>
     <row r="385" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A385" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="B385" s="4" t="s">
         <v>604</v>
-      </c>
-      <c r="B385" s="4" t="s">
-        <v>605</v>
       </c>
       <c r="C385" s="4"/>
       <c r="D385" s="2"/>
@@ -14423,11 +14423,11 @@
     </row>
     <row r="386" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A386" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B386" s="4"/>
       <c r="C386" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D386" s="2"/>
       <c r="E386" s="2"/>
@@ -14454,11 +14454,11 @@
     </row>
     <row r="387" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A387" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B387" s="4"/>
       <c r="C387" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D387" s="2"/>
       <c r="E387" s="2"/>
@@ -14485,7 +14485,7 @@
     </row>
     <row r="388" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A388" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B388" s="4"/>
       <c r="C388" s="4"/>
@@ -14514,7 +14514,7 @@
     </row>
     <row r="389" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A389" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B389" s="4"/>
       <c r="C389" s="4"/>
@@ -14543,7 +14543,7 @@
     </row>
     <row r="390" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A390" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B390" s="4"/>
       <c r="C390" s="4"/>
@@ -14572,10 +14572,10 @@
     </row>
     <row r="391" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A391" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="B391" s="4" t="s">
         <v>613</v>
-      </c>
-      <c r="B391" s="4" t="s">
-        <v>614</v>
       </c>
       <c r="C391" s="4"/>
       <c r="D391" s="2"/>
@@ -14603,11 +14603,11 @@
     </row>
     <row r="392" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A392" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B392" s="4"/>
       <c r="C392" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D392" s="2"/>
       <c r="E392" s="2"/>
@@ -14634,11 +14634,11 @@
     </row>
     <row r="393" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A393" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B393" s="4"/>
       <c r="C393" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D393" s="2"/>
       <c r="E393" s="2"/>
@@ -14665,10 +14665,10 @@
     </row>
     <row r="394" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A394" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="B394" s="4" t="s">
         <v>619</v>
-      </c>
-      <c r="B394" s="4" t="s">
-        <v>620</v>
       </c>
       <c r="C394" s="4"/>
       <c r="D394" s="2"/>
@@ -14696,11 +14696,11 @@
     </row>
     <row r="395" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A395" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B395" s="4"/>
       <c r="C395" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D395" s="2"/>
       <c r="E395" s="2"/>
@@ -14727,11 +14727,11 @@
     </row>
     <row r="396" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A396" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B396" s="4"/>
       <c r="C396" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D396" s="2"/>
       <c r="E396" s="2"/>
@@ -14758,11 +14758,11 @@
     </row>
     <row r="397" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A397" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B397" s="4"/>
       <c r="C397" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D397" s="2"/>
       <c r="E397" s="2"/>
@@ -14789,10 +14789,10 @@
     </row>
     <row r="398" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A398" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="B398" s="4" t="s">
         <v>627</v>
-      </c>
-      <c r="B398" s="4" t="s">
-        <v>628</v>
       </c>
       <c r="C398" s="4"/>
       <c r="D398" s="2"/>
@@ -14820,7 +14820,7 @@
     </row>
     <row r="399" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A399" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B399" s="4"/>
       <c r="C399" s="4"/>
@@ -14849,11 +14849,11 @@
     </row>
     <row r="400" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A400" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B400" s="4"/>
       <c r="C400" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D400" s="2"/>
       <c r="E400" s="2"/>
@@ -14880,10 +14880,10 @@
     </row>
     <row r="401" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A401" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="B401" s="4" t="s">
         <v>632</v>
-      </c>
-      <c r="B401" s="4" t="s">
-        <v>633</v>
       </c>
       <c r="C401" s="4"/>
       <c r="D401" s="2"/>
@@ -14911,11 +14911,11 @@
     </row>
     <row r="402" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A402" s="4" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B402" s="4"/>
       <c r="C402" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D402" s="2"/>
       <c r="E402" s="2"/>
@@ -14942,7 +14942,7 @@
     </row>
     <row r="403" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A403" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B403" s="4"/>
       <c r="C403" s="4"/>
@@ -14971,7 +14971,7 @@
     </row>
     <row r="404" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A404" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B404" s="4"/>
       <c r="C404" s="4"/>
@@ -15000,11 +15000,11 @@
     </row>
     <row r="405" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A405" s="4" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B405" s="4"/>
       <c r="C405" s="4" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D405" s="2"/>
       <c r="E405" s="2"/>
@@ -15031,7 +15031,7 @@
     </row>
     <row r="406" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A406" s="4" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B406" s="4"/>
       <c r="C406" s="4"/>
@@ -15060,11 +15060,11 @@
     </row>
     <row r="407" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A407" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B407" s="4"/>
       <c r="C407" s="4" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D407" s="2"/>
       <c r="E407" s="2"/>
@@ -15091,7 +15091,7 @@
     </row>
     <row r="408" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A408" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B408" s="4"/>
       <c r="C408" s="4"/>
@@ -15120,7 +15120,7 @@
     </row>
     <row r="409" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A409" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B409" s="4"/>
       <c r="C409" s="4"/>
@@ -15149,7 +15149,7 @@
     </row>
     <row r="410" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A410" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B410" s="4"/>
       <c r="C410" s="4"/>
@@ -15178,7 +15178,7 @@
     </row>
     <row r="411" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A411" s="4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B411" s="4"/>
       <c r="C411" s="4"/>
@@ -15207,10 +15207,10 @@
     </row>
     <row r="412" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A412" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="B412" s="4" t="s">
         <v>647</v>
-      </c>
-      <c r="B412" s="4" t="s">
-        <v>648</v>
       </c>
       <c r="C412" s="4"/>
       <c r="D412" s="2"/>
@@ -15238,7 +15238,7 @@
     </row>
     <row r="413" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A413" s="4" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B413" s="4"/>
       <c r="C413" s="4"/>
@@ -15267,7 +15267,7 @@
     </row>
     <row r="414" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A414" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B414" s="4"/>
       <c r="C414" s="4"/>
@@ -15296,7 +15296,7 @@
     </row>
     <row r="415" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A415" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B415" s="4"/>
       <c r="C415" s="4"/>
@@ -15325,7 +15325,7 @@
     </row>
     <row r="416" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A416" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B416" s="4"/>
       <c r="C416" s="4"/>
@@ -15354,7 +15354,7 @@
     </row>
     <row r="417" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A417" s="4" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B417" s="4"/>
       <c r="C417" s="4"/>
@@ -15383,7 +15383,7 @@
     </row>
     <row r="418" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A418" s="4" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B418" s="4"/>
       <c r="C418" s="2"/>
@@ -15412,7 +15412,7 @@
     </row>
     <row r="419" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A419" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B419" s="4"/>
       <c r="C419" s="2"/>
@@ -15441,7 +15441,7 @@
     </row>
     <row r="420" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A420" s="4" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B420" s="4"/>
       <c r="C420" s="2"/>
@@ -15470,10 +15470,10 @@
     </row>
     <row r="421" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A421" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="B421" s="4" t="s">
         <v>657</v>
-      </c>
-      <c r="B421" s="4" t="s">
-        <v>658</v>
       </c>
       <c r="C421" s="2"/>
       <c r="D421" s="2"/>

</xml_diff>

<commit_message>
Fix weird spacing wikipathway names
</commit_message>
<xml_diff>
--- a/mappings/wikipathways_reactome.xlsx
+++ b/mappings/wikipathways_reactome.xlsx
@@ -1263,9 +1263,6 @@
     <t>Lung fibrosis</t>
   </si>
   <si>
-    <t>MAPK and NFkB Signalling Pathways Inhibited by Yersinia YopJ</t>
-  </si>
-  <si>
     <t>MAPK Cascade</t>
   </si>
   <si>
@@ -2416,6 +2413,9 @@
   </si>
   <si>
     <t>H19 action Rb-E2F1 signaling and CDK-β-catenin activity</t>
+  </si>
+  <si>
+    <t>MAPK  and NFkB Signalling Pathways Inhibited by Yersinia YopJ</t>
   </si>
 </sst>
 </file>
@@ -2782,8 +2782,8 @@
   </sheetPr>
   <dimension ref="A1:Y999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="60" workbookViewId="0">
-      <selection activeCell="A159" sqref="A159"/>
+    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="60" workbookViewId="0">
+      <selection activeCell="A216" sqref="A216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2803,7 +2803,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -3010,7 +3010,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -4311,13 +4311,13 @@
     </row>
     <row r="51" spans="1:25" ht="409" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>658</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>659</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="122" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="4" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -7038,7 +7038,7 @@
         <v>223</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C141" s="4"/>
       <c r="D141" s="2"/>
@@ -7585,7 +7585,7 @@
     </row>
     <row r="159" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
@@ -8211,7 +8211,7 @@
         <v>281</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C180" s="4"/>
       <c r="D180" s="2"/>
@@ -9277,7 +9277,7 @@
     </row>
     <row r="215" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A215" s="4" t="s">
-        <v>342</v>
+        <v>668</v>
       </c>
       <c r="B215" s="4"/>
       <c r="C215" s="4"/>
@@ -9306,10 +9306,10 @@
     </row>
     <row r="216" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A216" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="B216" s="4" t="s">
         <v>343</v>
-      </c>
-      <c r="B216" s="4" t="s">
-        <v>344</v>
       </c>
       <c r="C216" s="4"/>
       <c r="D216" s="2"/>
@@ -9337,10 +9337,10 @@
     </row>
     <row r="217" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A217" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="B217" s="4" t="s">
         <v>345</v>
-      </c>
-      <c r="B217" s="4" t="s">
-        <v>346</v>
       </c>
       <c r="C217" s="4"/>
       <c r="D217" s="2"/>
@@ -9368,7 +9368,7 @@
     </row>
     <row r="218" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A218" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B218" s="4"/>
       <c r="C218" s="4"/>
@@ -9397,7 +9397,7 @@
     </row>
     <row r="219" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A219" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B219" s="4"/>
       <c r="C219" s="4"/>
@@ -9426,11 +9426,11 @@
     </row>
     <row r="220" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A220" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B220" s="4"/>
       <c r="C220" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
@@ -9457,11 +9457,11 @@
     </row>
     <row r="221" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A221" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B221" s="4"/>
       <c r="C221" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
@@ -9488,7 +9488,7 @@
     </row>
     <row r="222" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A222" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B222" s="4"/>
       <c r="C222" s="4"/>
@@ -9517,7 +9517,7 @@
     </row>
     <row r="223" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A223" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B223" s="4"/>
       <c r="C223" s="4"/>
@@ -9546,11 +9546,11 @@
     </row>
     <row r="224" spans="1:25" ht="130" x14ac:dyDescent="0.15">
       <c r="A224" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B224" s="4"/>
       <c r="C224" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
@@ -9577,11 +9577,11 @@
     </row>
     <row r="225" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A225" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B225" s="4"/>
       <c r="C225" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D225" s="2"/>
       <c r="E225" s="2"/>
@@ -9608,7 +9608,7 @@
     </row>
     <row r="226" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A226" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B226" s="4"/>
       <c r="C226" s="4"/>
@@ -9637,7 +9637,7 @@
     </row>
     <row r="227" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A227" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B227" s="4"/>
       <c r="C227" s="4"/>
@@ -9666,13 +9666,13 @@
     </row>
     <row r="228" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A228" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="B228" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="B228" s="4" t="s">
+      <c r="C228" s="4" t="s">
         <v>362</v>
-      </c>
-      <c r="C228" s="4" t="s">
-        <v>363</v>
       </c>
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
@@ -9699,10 +9699,10 @@
     </row>
     <row r="229" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A229" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="B229" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="B229" s="4" t="s">
-        <v>365</v>
       </c>
       <c r="C229" s="4"/>
       <c r="D229" s="2"/>
@@ -9730,7 +9730,7 @@
     </row>
     <row r="230" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A230" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B230" s="4"/>
       <c r="C230" s="4"/>
@@ -9759,11 +9759,11 @@
     </row>
     <row r="231" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A231" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B231" s="4"/>
       <c r="C231" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D231" s="2"/>
       <c r="E231" s="2"/>
@@ -9790,10 +9790,10 @@
     </row>
     <row r="232" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A232" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="B232" s="4" t="s">
         <v>369</v>
-      </c>
-      <c r="B232" s="4" t="s">
-        <v>370</v>
       </c>
       <c r="C232" s="4"/>
       <c r="D232" s="2"/>
@@ -9821,11 +9821,11 @@
     </row>
     <row r="233" spans="1:25" ht="221" x14ac:dyDescent="0.15">
       <c r="A233" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B233" s="4"/>
       <c r="C233" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
@@ -9852,11 +9852,11 @@
     </row>
     <row r="234" spans="1:25" ht="273" x14ac:dyDescent="0.15">
       <c r="A234" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B234" s="4"/>
       <c r="C234" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
@@ -9883,11 +9883,11 @@
     </row>
     <row r="235" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A235" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B235" s="4"/>
       <c r="C235" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D235" s="2"/>
       <c r="E235" s="2"/>
@@ -9914,11 +9914,11 @@
     </row>
     <row r="236" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A236" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B236" s="4"/>
       <c r="C236" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D236" s="2"/>
       <c r="E236" s="2"/>
@@ -9945,7 +9945,7 @@
     </row>
     <row r="237" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A237" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B237" s="4"/>
       <c r="C237" s="4"/>
@@ -9974,11 +9974,11 @@
     </row>
     <row r="238" spans="1:25" ht="169" x14ac:dyDescent="0.15">
       <c r="A238" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B238" s="4"/>
       <c r="C238" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
@@ -10005,7 +10005,7 @@
     </row>
     <row r="239" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A239" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B239" s="4"/>
       <c r="C239" s="4"/>
@@ -10034,11 +10034,11 @@
     </row>
     <row r="240" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A240" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B240" s="4"/>
       <c r="C240" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
@@ -10065,11 +10065,11 @@
     </row>
     <row r="241" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A241" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B241" s="4"/>
       <c r="C241" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D241" s="2"/>
       <c r="E241" s="2"/>
@@ -10096,11 +10096,11 @@
     </row>
     <row r="242" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A242" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B242" s="4"/>
       <c r="C242" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D242" s="2"/>
       <c r="E242" s="2"/>
@@ -10127,7 +10127,7 @@
     </row>
     <row r="243" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A243" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B243" s="4"/>
       <c r="C243" s="4"/>
@@ -10156,7 +10156,7 @@
     </row>
     <row r="244" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A244" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B244" s="4"/>
       <c r="C244" s="4"/>
@@ -10185,7 +10185,7 @@
     </row>
     <row r="245" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A245" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B245" s="4"/>
       <c r="C245" s="4"/>
@@ -10214,11 +10214,11 @@
     </row>
     <row r="246" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A246" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B246" s="4"/>
       <c r="C246" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D246" s="2"/>
       <c r="E246" s="2"/>
@@ -10245,7 +10245,7 @@
     </row>
     <row r="247" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A247" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B247" s="4"/>
       <c r="C247" s="4"/>
@@ -10274,11 +10274,11 @@
     </row>
     <row r="248" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A248" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B248" s="4"/>
       <c r="C248" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D248" s="2"/>
       <c r="E248" s="2"/>
@@ -10305,7 +10305,7 @@
     </row>
     <row r="249" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A249" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B249" s="4"/>
       <c r="C249" s="4"/>
@@ -10334,7 +10334,7 @@
     </row>
     <row r="250" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A250" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B250" s="4"/>
       <c r="C250" s="4"/>
@@ -10363,11 +10363,11 @@
     </row>
     <row r="251" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A251" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B251" s="4"/>
       <c r="C251" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D251" s="2"/>
       <c r="E251" s="2"/>
@@ -10394,7 +10394,7 @@
     </row>
     <row r="252" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A252" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B252" s="4"/>
       <c r="C252" s="4"/>
@@ -10423,11 +10423,11 @@
     </row>
     <row r="253" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A253" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B253" s="4"/>
       <c r="C253" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D253" s="2"/>
       <c r="E253" s="2"/>
@@ -10454,11 +10454,11 @@
     </row>
     <row r="254" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A254" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B254" s="4"/>
       <c r="C254" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D254" s="2"/>
       <c r="E254" s="2"/>
@@ -10485,10 +10485,10 @@
     </row>
     <row r="255" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A255" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B255" s="4" t="s">
         <v>406</v>
-      </c>
-      <c r="B255" s="4" t="s">
-        <v>407</v>
       </c>
       <c r="C255" s="4"/>
       <c r="D255" s="2"/>
@@ -10516,10 +10516,10 @@
     </row>
     <row r="256" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A256" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="B256" s="4" t="s">
         <v>408</v>
-      </c>
-      <c r="B256" s="4" t="s">
-        <v>409</v>
       </c>
       <c r="C256" s="4"/>
       <c r="D256" s="2"/>
@@ -10547,11 +10547,11 @@
     </row>
     <row r="257" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A257" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B257" s="4"/>
       <c r="C257" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D257" s="2"/>
       <c r="E257" s="2"/>
@@ -10578,11 +10578,11 @@
     </row>
     <row r="258" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A258" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B258" s="4"/>
       <c r="C258" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D258" s="2"/>
       <c r="E258" s="2"/>
@@ -10609,7 +10609,7 @@
     </row>
     <row r="259" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A259" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B259" s="4"/>
       <c r="C259" s="4"/>
@@ -10638,10 +10638,10 @@
     </row>
     <row r="260" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A260" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B260" s="4" t="s">
         <v>415</v>
-      </c>
-      <c r="B260" s="4" t="s">
-        <v>416</v>
       </c>
       <c r="C260" s="4"/>
       <c r="D260" s="2"/>
@@ -10669,7 +10669,7 @@
     </row>
     <row r="261" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A261" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B261" s="4"/>
       <c r="C261" s="4"/>
@@ -10698,7 +10698,7 @@
     </row>
     <row r="262" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A262" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B262" s="4"/>
       <c r="C262" s="4"/>
@@ -10727,11 +10727,11 @@
     </row>
     <row r="263" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A263" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B263" s="4"/>
       <c r="C263" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D263" s="2"/>
       <c r="E263" s="2"/>
@@ -10758,11 +10758,11 @@
     </row>
     <row r="264" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A264" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B264" s="4"/>
       <c r="C264" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D264" s="2"/>
       <c r="E264" s="2"/>
@@ -10789,11 +10789,11 @@
     </row>
     <row r="265" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A265" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B265" s="4"/>
       <c r="C265" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D265" s="2"/>
       <c r="E265" s="2"/>
@@ -10820,7 +10820,7 @@
     </row>
     <row r="266" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A266" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B266" s="4"/>
       <c r="C266" s="4"/>
@@ -10849,7 +10849,7 @@
     </row>
     <row r="267" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A267" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B267" s="4"/>
       <c r="C267" s="4"/>
@@ -10878,7 +10878,7 @@
     </row>
     <row r="268" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A268" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B268" s="4"/>
       <c r="C268" s="4"/>
@@ -10907,7 +10907,7 @@
     </row>
     <row r="269" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A269" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B269" s="4"/>
       <c r="C269" s="4"/>
@@ -10936,7 +10936,7 @@
     </row>
     <row r="270" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A270" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B270" s="4"/>
       <c r="C270" s="4"/>
@@ -10965,11 +10965,11 @@
     </row>
     <row r="271" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A271" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B271" s="4"/>
       <c r="C271" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D271" s="2"/>
       <c r="E271" s="2"/>
@@ -10996,11 +10996,11 @@
     </row>
     <row r="272" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A272" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B272" s="4"/>
       <c r="C272" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D272" s="2"/>
       <c r="E272" s="2"/>
@@ -11027,11 +11027,11 @@
     </row>
     <row r="273" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A273" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B273" s="4"/>
       <c r="C273" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D273" s="2"/>
       <c r="E273" s="2"/>
@@ -11058,10 +11058,10 @@
     </row>
     <row r="274" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A274" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="B274" s="4" t="s">
         <v>436</v>
-      </c>
-      <c r="B274" s="4" t="s">
-        <v>437</v>
       </c>
       <c r="C274" s="4"/>
       <c r="D274" s="2"/>
@@ -11089,7 +11089,7 @@
     </row>
     <row r="275" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A275" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B275" s="4"/>
       <c r="C275" s="4"/>
@@ -11118,11 +11118,11 @@
     </row>
     <row r="276" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A276" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B276" s="4"/>
       <c r="C276" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D276" s="2"/>
       <c r="E276" s="2"/>
@@ -11149,7 +11149,7 @@
     </row>
     <row r="277" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A277" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B277" s="4"/>
       <c r="C277" s="4"/>
@@ -11178,11 +11178,11 @@
     </row>
     <row r="278" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A278" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B278" s="4"/>
       <c r="C278" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D278" s="2"/>
       <c r="E278" s="2"/>
@@ -11209,10 +11209,10 @@
     </row>
     <row r="279" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A279" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="B279" s="4" t="s">
         <v>444</v>
-      </c>
-      <c r="B279" s="4" t="s">
-        <v>445</v>
       </c>
       <c r="C279" s="4"/>
       <c r="D279" s="2"/>
@@ -11240,7 +11240,7 @@
     </row>
     <row r="280" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A280" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B280" s="4"/>
       <c r="C280" s="4"/>
@@ -11269,11 +11269,11 @@
     </row>
     <row r="281" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A281" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B281" s="4"/>
       <c r="C281" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D281" s="2"/>
       <c r="E281" s="2"/>
@@ -11300,11 +11300,11 @@
     </row>
     <row r="282" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A282" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B282" s="4"/>
       <c r="C282" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D282" s="2"/>
       <c r="E282" s="2"/>
@@ -11331,7 +11331,7 @@
     </row>
     <row r="283" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A283" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B283" s="4"/>
       <c r="C283" s="4"/>
@@ -11360,7 +11360,7 @@
     </row>
     <row r="284" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A284" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B284" s="4"/>
       <c r="C284" s="4"/>
@@ -11389,11 +11389,11 @@
     </row>
     <row r="285" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A285" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B285" s="4"/>
       <c r="C285" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D285" s="2"/>
       <c r="E285" s="2"/>
@@ -11420,11 +11420,11 @@
     </row>
     <row r="286" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A286" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B286" s="4"/>
       <c r="C286" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D286" s="2"/>
       <c r="E286" s="2"/>
@@ -11451,7 +11451,7 @@
     </row>
     <row r="287" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A287" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B287" s="4"/>
       <c r="C287" s="4"/>
@@ -11480,10 +11480,10 @@
     </row>
     <row r="288" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A288" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="B288" s="4" t="s">
         <v>458</v>
-      </c>
-      <c r="B288" s="4" t="s">
-        <v>459</v>
       </c>
       <c r="C288" s="4"/>
       <c r="D288" s="2"/>
@@ -11511,11 +11511,11 @@
     </row>
     <row r="289" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A289" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B289" s="4"/>
       <c r="C289" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D289" s="2"/>
       <c r="E289" s="2"/>
@@ -11542,11 +11542,11 @@
     </row>
     <row r="290" spans="1:25" ht="130" x14ac:dyDescent="0.15">
       <c r="A290" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B290" s="4"/>
       <c r="C290" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D290" s="2"/>
       <c r="E290" s="2"/>
@@ -11573,11 +11573,11 @@
     </row>
     <row r="291" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A291" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B291" s="4"/>
       <c r="C291" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D291" s="2"/>
       <c r="E291" s="2"/>
@@ -11604,7 +11604,7 @@
     </row>
     <row r="292" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A292" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B292" s="4"/>
       <c r="C292" s="4"/>
@@ -11633,7 +11633,7 @@
     </row>
     <row r="293" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A293" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B293" s="4"/>
       <c r="C293" s="4"/>
@@ -11662,7 +11662,7 @@
     </row>
     <row r="294" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A294" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B294" s="4"/>
       <c r="C294" s="4"/>
@@ -11691,7 +11691,7 @@
     </row>
     <row r="295" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A295" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B295" s="4"/>
       <c r="C295" s="4"/>
@@ -11720,7 +11720,7 @@
     </row>
     <row r="296" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A296" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B296" s="4"/>
       <c r="C296" s="4"/>
@@ -11749,7 +11749,7 @@
     </row>
     <row r="297" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A297" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B297" s="4"/>
       <c r="C297" s="4"/>
@@ -11778,11 +11778,11 @@
     </row>
     <row r="298" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A298" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B298" s="4"/>
       <c r="C298" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D298" s="2"/>
       <c r="E298" s="2"/>
@@ -11809,7 +11809,7 @@
     </row>
     <row r="299" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A299" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B299" s="4"/>
       <c r="C299" s="4"/>
@@ -11838,7 +11838,7 @@
     </row>
     <row r="300" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A300" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B300" s="4"/>
       <c r="C300" s="4"/>
@@ -11867,7 +11867,7 @@
     </row>
     <row r="301" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A301" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B301" s="4"/>
       <c r="C301" s="4"/>
@@ -11896,7 +11896,7 @@
     </row>
     <row r="302" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A302" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B302" s="4"/>
       <c r="C302" s="4"/>
@@ -11925,7 +11925,7 @@
     </row>
     <row r="303" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A303" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B303" s="4"/>
       <c r="C303" s="4"/>
@@ -11954,10 +11954,10 @@
     </row>
     <row r="304" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A304" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="B304" s="4" t="s">
         <v>479</v>
-      </c>
-      <c r="B304" s="4" t="s">
-        <v>480</v>
       </c>
       <c r="C304" s="4"/>
       <c r="D304" s="2"/>
@@ -11985,7 +11985,7 @@
     </row>
     <row r="305" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A305" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B305" s="4"/>
       <c r="C305" s="4"/>
@@ -12014,11 +12014,11 @@
     </row>
     <row r="306" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A306" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B306" s="4"/>
       <c r="C306" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D306" s="2"/>
       <c r="E306" s="2"/>
@@ -12045,11 +12045,11 @@
     </row>
     <row r="307" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A307" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B307" s="4"/>
       <c r="C307" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D307" s="2"/>
       <c r="E307" s="2"/>
@@ -12076,11 +12076,11 @@
     </row>
     <row r="308" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A308" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B308" s="4"/>
       <c r="C308" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D308" s="2"/>
       <c r="E308" s="2"/>
@@ -12107,7 +12107,7 @@
     </row>
     <row r="309" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A309" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B309" s="4"/>
       <c r="C309" s="4"/>
@@ -12136,11 +12136,11 @@
     </row>
     <row r="310" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A310" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B310" s="4"/>
       <c r="C310" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D310" s="2"/>
       <c r="E310" s="2"/>
@@ -12167,7 +12167,7 @@
     </row>
     <row r="311" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A311" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B311" s="4"/>
       <c r="C311" s="4"/>
@@ -12196,11 +12196,11 @@
     </row>
     <row r="312" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A312" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B312" s="4"/>
       <c r="C312" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D312" s="2"/>
       <c r="E312" s="2"/>
@@ -12227,7 +12227,7 @@
     </row>
     <row r="313" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A313" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B313" s="4"/>
       <c r="C313" s="4"/>
@@ -12256,7 +12256,7 @@
     </row>
     <row r="314" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A314" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B314" s="4"/>
       <c r="C314" s="4"/>
@@ -12285,11 +12285,11 @@
     </row>
     <row r="315" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A315" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B315" s="4"/>
       <c r="C315" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D315" s="2"/>
       <c r="E315" s="2"/>
@@ -12316,7 +12316,7 @@
     </row>
     <row r="316" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A316" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B316" s="4"/>
       <c r="C316" s="4"/>
@@ -12345,11 +12345,11 @@
     </row>
     <row r="317" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A317" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B317" s="4"/>
       <c r="C317" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D317" s="2"/>
       <c r="E317" s="2"/>
@@ -12376,11 +12376,11 @@
     </row>
     <row r="318" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A318" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B318" s="4"/>
       <c r="C318" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D318" s="2"/>
       <c r="E318" s="2"/>
@@ -12407,7 +12407,7 @@
     </row>
     <row r="319" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A319" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B319" s="4"/>
       <c r="C319" s="4"/>
@@ -12436,11 +12436,11 @@
     </row>
     <row r="320" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A320" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B320" s="4"/>
       <c r="C320" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D320" s="2"/>
       <c r="E320" s="2"/>
@@ -12467,7 +12467,7 @@
     </row>
     <row r="321" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A321" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B321" s="4"/>
       <c r="C321" s="4"/>
@@ -12496,7 +12496,7 @@
     </row>
     <row r="322" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A322" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B322" s="4"/>
       <c r="C322" s="4"/>
@@ -12525,11 +12525,11 @@
     </row>
     <row r="323" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A323" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B323" s="4"/>
       <c r="C323" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D323" s="2"/>
       <c r="E323" s="2"/>
@@ -12556,7 +12556,7 @@
     </row>
     <row r="324" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A324" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B324" s="4"/>
       <c r="C324" s="4"/>
@@ -12585,7 +12585,7 @@
     </row>
     <row r="325" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A325" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B325" s="4"/>
       <c r="C325" s="4"/>
@@ -12614,11 +12614,11 @@
     </row>
     <row r="326" spans="1:25" ht="143" x14ac:dyDescent="0.15">
       <c r="A326" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B326" s="4"/>
       <c r="C326" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D326" s="2"/>
       <c r="E326" s="2"/>
@@ -12645,11 +12645,11 @@
     </row>
     <row r="327" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A327" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B327" s="4"/>
       <c r="C327" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D327" s="2"/>
       <c r="E327" s="2"/>
@@ -12676,7 +12676,7 @@
     </row>
     <row r="328" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A328" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B328" s="4"/>
       <c r="C328" s="4"/>
@@ -12705,11 +12705,11 @@
     </row>
     <row r="329" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A329" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B329" s="4"/>
       <c r="C329" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D329" s="2"/>
       <c r="E329" s="2"/>
@@ -12736,7 +12736,7 @@
     </row>
     <row r="330" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A330" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B330" s="4"/>
       <c r="D330" s="2"/>
@@ -12764,11 +12764,11 @@
     </row>
     <row r="331" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A331" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B331" s="4"/>
       <c r="C331" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D331" s="2"/>
       <c r="E331" s="2"/>
@@ -12795,11 +12795,11 @@
     </row>
     <row r="332" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A332" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B332" s="4"/>
       <c r="C332" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D332" s="2"/>
       <c r="E332" s="2"/>
@@ -12826,7 +12826,7 @@
     </row>
     <row r="333" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A333" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B333" s="4"/>
       <c r="C333" s="4"/>
@@ -12855,7 +12855,7 @@
     </row>
     <row r="334" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A334" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B334" s="4"/>
       <c r="C334" s="4"/>
@@ -12884,11 +12884,11 @@
     </row>
     <row r="335" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A335" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B335" s="4"/>
       <c r="C335" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D335" s="2"/>
       <c r="E335" s="2"/>
@@ -12915,7 +12915,7 @@
     </row>
     <row r="336" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A336" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B336" s="4"/>
       <c r="C336" s="4"/>
@@ -12944,7 +12944,7 @@
     </row>
     <row r="337" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A337" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B337" s="4"/>
       <c r="C337" s="4"/>
@@ -12973,11 +12973,11 @@
     </row>
     <row r="338" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A338" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B338" s="4"/>
       <c r="C338" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D338" s="2"/>
       <c r="E338" s="2"/>
@@ -13004,7 +13004,7 @@
     </row>
     <row r="339" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A339" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B339" s="4"/>
       <c r="C339" s="4"/>
@@ -13033,11 +13033,11 @@
     </row>
     <row r="340" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A340" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B340" s="4"/>
       <c r="C340" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D340" s="2"/>
       <c r="E340" s="2"/>
@@ -13064,7 +13064,7 @@
     </row>
     <row r="341" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A341" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B341" s="4"/>
       <c r="C341" s="4"/>
@@ -13093,10 +13093,10 @@
     </row>
     <row r="342" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A342" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="B342" s="4" t="s">
         <v>536</v>
-      </c>
-      <c r="B342" s="4" t="s">
-        <v>537</v>
       </c>
       <c r="C342" s="4"/>
       <c r="D342" s="2"/>
@@ -13124,7 +13124,7 @@
     </row>
     <row r="343" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A343" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B343" s="4"/>
       <c r="C343" s="4"/>
@@ -13153,7 +13153,7 @@
     </row>
     <row r="344" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A344" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B344" s="4"/>
       <c r="C344" s="4"/>
@@ -13182,7 +13182,7 @@
     </row>
     <row r="345" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A345" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B345" s="4"/>
       <c r="C345" s="4"/>
@@ -13211,11 +13211,11 @@
     </row>
     <row r="346" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A346" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B346" s="4"/>
       <c r="C346" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D346" s="2"/>
       <c r="E346" s="2"/>
@@ -13242,11 +13242,11 @@
     </row>
     <row r="347" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A347" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B347" s="4"/>
       <c r="C347" s="4" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D347" s="2"/>
       <c r="E347" s="2"/>
@@ -13273,10 +13273,10 @@
     </row>
     <row r="348" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A348" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="B348" s="4" t="s">
         <v>545</v>
-      </c>
-      <c r="B348" s="4" t="s">
-        <v>546</v>
       </c>
       <c r="C348" s="4"/>
       <c r="D348" s="2"/>
@@ -13304,11 +13304,11 @@
     </row>
     <row r="349" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A349" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B349" s="4"/>
       <c r="C349" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D349" s="2"/>
       <c r="E349" s="2"/>
@@ -13335,7 +13335,7 @@
     </row>
     <row r="350" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A350" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B350" s="4"/>
       <c r="C350" s="4"/>
@@ -13364,11 +13364,11 @@
     </row>
     <row r="351" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A351" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B351" s="4"/>
       <c r="C351" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D351" s="2"/>
       <c r="E351" s="2"/>
@@ -13395,7 +13395,7 @@
     </row>
     <row r="352" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A352" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B352" s="4"/>
       <c r="C352" s="4"/>
@@ -13424,11 +13424,11 @@
     </row>
     <row r="353" spans="1:25" ht="143" x14ac:dyDescent="0.15">
       <c r="A353" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B353" s="4"/>
       <c r="C353" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D353" s="2"/>
       <c r="E353" s="2"/>
@@ -13455,10 +13455,10 @@
     </row>
     <row r="354" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A354" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="B354" s="4" t="s">
         <v>555</v>
-      </c>
-      <c r="B354" s="4" t="s">
-        <v>556</v>
       </c>
       <c r="C354" s="4"/>
       <c r="D354" s="2"/>
@@ -13486,11 +13486,11 @@
     </row>
     <row r="355" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A355" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B355" s="4"/>
       <c r="C355" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D355" s="2"/>
       <c r="E355" s="2"/>
@@ -13517,11 +13517,11 @@
     </row>
     <row r="356" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A356" s="4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B356" s="4"/>
       <c r="C356" s="4" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D356" s="2"/>
       <c r="E356" s="2"/>
@@ -13548,7 +13548,7 @@
     </row>
     <row r="357" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A357" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B357" s="4"/>
       <c r="C357" s="4"/>
@@ -13577,10 +13577,10 @@
     </row>
     <row r="358" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A358" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="B358" s="4" t="s">
         <v>560</v>
-      </c>
-      <c r="B358" s="4" t="s">
-        <v>561</v>
       </c>
       <c r="C358" s="4"/>
       <c r="D358" s="2"/>
@@ -13608,7 +13608,7 @@
     </row>
     <row r="359" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A359" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B359" s="4"/>
       <c r="C359" s="4"/>
@@ -13637,7 +13637,7 @@
     </row>
     <row r="360" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A360" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B360" s="4"/>
       <c r="C360" s="4"/>
@@ -13666,7 +13666,7 @@
     </row>
     <row r="361" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A361" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B361" s="4"/>
       <c r="C361" s="4"/>
@@ -13695,10 +13695,10 @@
     </row>
     <row r="362" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A362" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B362" s="4" t="s">
         <v>565</v>
-      </c>
-      <c r="B362" s="4" t="s">
-        <v>566</v>
       </c>
       <c r="C362" s="4"/>
       <c r="D362" s="2"/>
@@ -13726,10 +13726,10 @@
     </row>
     <row r="363" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A363" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="B363" s="4" t="s">
         <v>567</v>
-      </c>
-      <c r="B363" s="4" t="s">
-        <v>568</v>
       </c>
       <c r="C363" s="4"/>
       <c r="D363" s="2"/>
@@ -13757,10 +13757,10 @@
     </row>
     <row r="364" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A364" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="B364" s="4" t="s">
         <v>569</v>
-      </c>
-      <c r="B364" s="4" t="s">
-        <v>570</v>
       </c>
       <c r="C364" s="4"/>
       <c r="D364" s="2"/>
@@ -13788,11 +13788,11 @@
     </row>
     <row r="365" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A365" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B365" s="4"/>
       <c r="C365" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D365" s="2"/>
       <c r="E365" s="2"/>
@@ -13819,7 +13819,7 @@
     </row>
     <row r="366" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A366" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B366" s="4"/>
       <c r="C366" s="4"/>
@@ -13848,7 +13848,7 @@
     </row>
     <row r="367" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A367" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B367" s="4"/>
       <c r="C367" s="4"/>
@@ -13877,7 +13877,7 @@
     </row>
     <row r="368" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A368" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B368" s="4"/>
       <c r="C368" s="4"/>
@@ -13906,7 +13906,7 @@
     </row>
     <row r="369" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A369" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B369" s="4"/>
       <c r="C369" s="4"/>
@@ -13935,11 +13935,11 @@
     </row>
     <row r="370" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A370" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B370" s="4"/>
       <c r="C370" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D370" s="2"/>
       <c r="E370" s="2"/>
@@ -13966,7 +13966,7 @@
     </row>
     <row r="371" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A371" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B371" s="4"/>
       <c r="C371" s="4"/>
@@ -13995,10 +13995,10 @@
     </row>
     <row r="372" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A372" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="B372" s="4" t="s">
         <v>580</v>
-      </c>
-      <c r="B372" s="4" t="s">
-        <v>581</v>
       </c>
       <c r="C372" s="4"/>
       <c r="D372" s="2"/>
@@ -14026,7 +14026,7 @@
     </row>
     <row r="373" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A373" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B373" s="4"/>
       <c r="C373" s="4"/>
@@ -14055,7 +14055,7 @@
     </row>
     <row r="374" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A374" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B374" s="4"/>
       <c r="C374" s="4"/>
@@ -14084,7 +14084,7 @@
     </row>
     <row r="375" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A375" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B375" s="4"/>
       <c r="C375" s="4"/>
@@ -14113,10 +14113,10 @@
     </row>
     <row r="376" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A376" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="B376" s="4" t="s">
         <v>585</v>
-      </c>
-      <c r="B376" s="4" t="s">
-        <v>586</v>
       </c>
       <c r="C376" s="4"/>
       <c r="D376" s="2"/>
@@ -14144,10 +14144,10 @@
     </row>
     <row r="377" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A377" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="B377" s="4" t="s">
         <v>587</v>
-      </c>
-      <c r="B377" s="4" t="s">
-        <v>588</v>
       </c>
       <c r="C377" s="4"/>
       <c r="D377" s="2"/>
@@ -14175,10 +14175,10 @@
     </row>
     <row r="378" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A378" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="B378" s="4" t="s">
         <v>589</v>
-      </c>
-      <c r="B378" s="4" t="s">
-        <v>590</v>
       </c>
       <c r="C378" s="4"/>
       <c r="D378" s="2"/>
@@ -14206,11 +14206,11 @@
     </row>
     <row r="379" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A379" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B379" s="4"/>
       <c r="C379" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D379" s="2"/>
       <c r="E379" s="2"/>
@@ -14237,13 +14237,13 @@
     </row>
     <row r="380" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A380" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="B380" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="B380" s="4" t="s">
+      <c r="C380" s="4" t="s">
         <v>594</v>
-      </c>
-      <c r="C380" s="4" t="s">
-        <v>595</v>
       </c>
       <c r="D380" s="2"/>
       <c r="E380" s="2"/>
@@ -14270,11 +14270,11 @@
     </row>
     <row r="381" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A381" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B381" s="4"/>
       <c r="C381" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D381" s="2"/>
       <c r="E381" s="2"/>
@@ -14301,7 +14301,7 @@
     </row>
     <row r="382" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A382" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B382" s="4"/>
       <c r="C382" s="4"/>
@@ -14330,11 +14330,11 @@
     </row>
     <row r="383" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A383" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B383" s="4"/>
       <c r="C383" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D383" s="2"/>
       <c r="E383" s="2"/>
@@ -14361,11 +14361,11 @@
     </row>
     <row r="384" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A384" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B384" s="4"/>
       <c r="C384" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D384" s="2"/>
       <c r="E384" s="2"/>
@@ -14392,10 +14392,10 @@
     </row>
     <row r="385" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A385" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="B385" s="4" t="s">
         <v>603</v>
-      </c>
-      <c r="B385" s="4" t="s">
-        <v>604</v>
       </c>
       <c r="C385" s="4"/>
       <c r="D385" s="2"/>
@@ -14423,11 +14423,11 @@
     </row>
     <row r="386" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A386" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B386" s="4"/>
       <c r="C386" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D386" s="2"/>
       <c r="E386" s="2"/>
@@ -14454,11 +14454,11 @@
     </row>
     <row r="387" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A387" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B387" s="4"/>
       <c r="C387" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D387" s="2"/>
       <c r="E387" s="2"/>
@@ -14485,7 +14485,7 @@
     </row>
     <row r="388" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A388" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B388" s="4"/>
       <c r="C388" s="4"/>
@@ -14514,7 +14514,7 @@
     </row>
     <row r="389" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A389" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B389" s="4"/>
       <c r="C389" s="4"/>
@@ -14543,7 +14543,7 @@
     </row>
     <row r="390" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A390" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B390" s="4"/>
       <c r="C390" s="4"/>
@@ -14572,10 +14572,10 @@
     </row>
     <row r="391" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A391" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="B391" s="4" t="s">
         <v>612</v>
-      </c>
-      <c r="B391" s="4" t="s">
-        <v>613</v>
       </c>
       <c r="C391" s="4"/>
       <c r="D391" s="2"/>
@@ -14603,11 +14603,11 @@
     </row>
     <row r="392" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A392" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B392" s="4"/>
       <c r="C392" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D392" s="2"/>
       <c r="E392" s="2"/>
@@ -14634,11 +14634,11 @@
     </row>
     <row r="393" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A393" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B393" s="4"/>
       <c r="C393" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D393" s="2"/>
       <c r="E393" s="2"/>
@@ -14665,10 +14665,10 @@
     </row>
     <row r="394" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A394" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="B394" s="4" t="s">
         <v>618</v>
-      </c>
-      <c r="B394" s="4" t="s">
-        <v>619</v>
       </c>
       <c r="C394" s="4"/>
       <c r="D394" s="2"/>
@@ -14696,11 +14696,11 @@
     </row>
     <row r="395" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A395" s="4" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B395" s="4"/>
       <c r="C395" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D395" s="2"/>
       <c r="E395" s="2"/>
@@ -14727,11 +14727,11 @@
     </row>
     <row r="396" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A396" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B396" s="4"/>
       <c r="C396" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D396" s="2"/>
       <c r="E396" s="2"/>
@@ -14758,11 +14758,11 @@
     </row>
     <row r="397" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A397" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B397" s="4"/>
       <c r="C397" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D397" s="2"/>
       <c r="E397" s="2"/>
@@ -14789,10 +14789,10 @@
     </row>
     <row r="398" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A398" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="B398" s="4" t="s">
         <v>626</v>
-      </c>
-      <c r="B398" s="4" t="s">
-        <v>627</v>
       </c>
       <c r="C398" s="4"/>
       <c r="D398" s="2"/>
@@ -14820,7 +14820,7 @@
     </row>
     <row r="399" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A399" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B399" s="4"/>
       <c r="C399" s="4"/>
@@ -14849,11 +14849,11 @@
     </row>
     <row r="400" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A400" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B400" s="4"/>
       <c r="C400" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D400" s="2"/>
       <c r="E400" s="2"/>
@@ -14880,10 +14880,10 @@
     </row>
     <row r="401" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A401" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="B401" s="4" t="s">
         <v>631</v>
-      </c>
-      <c r="B401" s="4" t="s">
-        <v>632</v>
       </c>
       <c r="C401" s="4"/>
       <c r="D401" s="2"/>
@@ -14911,11 +14911,11 @@
     </row>
     <row r="402" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A402" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B402" s="4"/>
       <c r="C402" s="4" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D402" s="2"/>
       <c r="E402" s="2"/>
@@ -14942,7 +14942,7 @@
     </row>
     <row r="403" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A403" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B403" s="4"/>
       <c r="C403" s="4"/>
@@ -14971,7 +14971,7 @@
     </row>
     <row r="404" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A404" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B404" s="4"/>
       <c r="C404" s="4"/>
@@ -15000,11 +15000,11 @@
     </row>
     <row r="405" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A405" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B405" s="4"/>
       <c r="C405" s="4" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D405" s="2"/>
       <c r="E405" s="2"/>
@@ -15031,7 +15031,7 @@
     </row>
     <row r="406" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A406" s="4" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B406" s="4"/>
       <c r="C406" s="4"/>
@@ -15060,11 +15060,11 @@
     </row>
     <row r="407" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A407" s="4" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B407" s="4"/>
       <c r="C407" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D407" s="2"/>
       <c r="E407" s="2"/>
@@ -15091,7 +15091,7 @@
     </row>
     <row r="408" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A408" s="4" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B408" s="4"/>
       <c r="C408" s="4"/>
@@ -15120,7 +15120,7 @@
     </row>
     <row r="409" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A409" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B409" s="4"/>
       <c r="C409" s="4"/>
@@ -15149,7 +15149,7 @@
     </row>
     <row r="410" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A410" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B410" s="4"/>
       <c r="C410" s="4"/>
@@ -15178,7 +15178,7 @@
     </row>
     <row r="411" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A411" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B411" s="4"/>
       <c r="C411" s="4"/>
@@ -15207,10 +15207,10 @@
     </row>
     <row r="412" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A412" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="B412" s="4" t="s">
         <v>646</v>
-      </c>
-      <c r="B412" s="4" t="s">
-        <v>647</v>
       </c>
       <c r="C412" s="4"/>
       <c r="D412" s="2"/>
@@ -15238,7 +15238,7 @@
     </row>
     <row r="413" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A413" s="4" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B413" s="4"/>
       <c r="C413" s="4"/>
@@ -15267,7 +15267,7 @@
     </row>
     <row r="414" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A414" s="4" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B414" s="4"/>
       <c r="C414" s="4"/>
@@ -15296,7 +15296,7 @@
     </row>
     <row r="415" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A415" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B415" s="4"/>
       <c r="C415" s="4"/>
@@ -15325,7 +15325,7 @@
     </row>
     <row r="416" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A416" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B416" s="4"/>
       <c r="C416" s="4"/>
@@ -15354,7 +15354,7 @@
     </row>
     <row r="417" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A417" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B417" s="4"/>
       <c r="C417" s="4"/>
@@ -15383,7 +15383,7 @@
     </row>
     <row r="418" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A418" s="4" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B418" s="4"/>
       <c r="C418" s="2"/>
@@ -15412,7 +15412,7 @@
     </row>
     <row r="419" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A419" s="4" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B419" s="4"/>
       <c r="C419" s="2"/>
@@ -15441,7 +15441,7 @@
     </row>
     <row r="420" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A420" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B420" s="4"/>
       <c r="C420" s="2"/>
@@ -15470,10 +15470,10 @@
     </row>
     <row r="421" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A421" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="B421" s="4" t="s">
         <v>656</v>
-      </c>
-      <c r="B421" s="4" t="s">
-        <v>657</v>
       </c>
       <c r="C421" s="2"/>
       <c r="D421" s="2"/>

</xml_diff>

<commit_message>
Clean wikipathway reactome encoding and weird spacings
</commit_message>
<xml_diff>
--- a/mappings/wikipathways_reactome.xlsx
+++ b/mappings/wikipathways_reactome.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1717,9 +1717,6 @@
     <t>Photodynamic therapy-induced unfolded protein response</t>
   </si>
   <si>
-    <t>Physiological and Pathological Hypertrophy of the Heart</t>
-  </si>
-  <si>
     <t>Polyol Pathway</t>
   </si>
   <si>
@@ -2197,9 +2194,6 @@
   </si>
   <si>
     <t>Tumor suppressor activity of SMARCB1</t>
-  </si>
-  <si>
-    <t>Type 1 Papillary Renal Cell Carcinoma</t>
   </si>
   <si>
     <t>Type II diabetes mellitus</t>
@@ -2316,9 +2310,6 @@
 mRNA Splicing - Minor Pathway isPartOf mRNA Processing*
 Processing of Capped Intron-Containing Pre-mRNA isPartOf mRNA Processing*
 Processing of Intronless Pre-mRNAs isPartOf mRNA Processing*</t>
-  </si>
-  <si>
-    <t>miR-148a/miR-31/FIH1/HIF1��-Notch signaling in glioblastoma</t>
   </si>
   <si>
     <t>miR-222 in Exercise-Induced Cardiac Growth</t>
@@ -2417,12 +2408,21 @@
   <si>
     <t>MAPK  and NFkB Signalling Pathways Inhibited by Yersinia YopJ</t>
   </si>
+  <si>
+    <t>Physiological and Pathological Hypertrophy  of the Heart</t>
+  </si>
+  <si>
+    <t>MET in type 1 papillary renal cell carcinoma</t>
+  </si>
+  <si>
+    <t>miR-148a/miR-31/FIH1/HIF1α-Notch signaling in glioblastoma</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2445,6 +2445,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2480,7 +2485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2500,6 +2505,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2782,8 +2788,8 @@
   </sheetPr>
   <dimension ref="A1:Y999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="60" workbookViewId="0">
-      <selection activeCell="A216" sqref="A216"/>
+    <sheetView tabSelected="1" topLeftCell="A397" zoomScale="60" workbookViewId="0">
+      <selection activeCell="A408" sqref="A408"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2803,7 +2809,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -3010,7 +3016,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -4311,13 +4317,13 @@
     </row>
     <row r="51" spans="1:25" ht="409" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -6452,7 +6458,7 @@
     </row>
     <row r="122" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="4" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -7038,7 +7044,7 @@
         <v>223</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C141" s="4"/>
       <c r="D141" s="2"/>
@@ -7585,7 +7591,7 @@
     </row>
     <row r="159" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="4" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
@@ -8211,7 +8217,7 @@
         <v>281</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C180" s="4"/>
       <c r="D180" s="2"/>
@@ -9277,7 +9283,7 @@
     </row>
     <row r="215" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A215" s="4" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="B215" s="4"/>
       <c r="C215" s="4"/>
@@ -11749,7 +11755,7 @@
     </row>
     <row r="297" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A297" s="4" t="s">
-        <v>470</v>
+        <v>666</v>
       </c>
       <c r="B297" s="4"/>
       <c r="C297" s="4"/>
@@ -11778,11 +11784,11 @@
     </row>
     <row r="298" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A298" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B298" s="4"/>
       <c r="C298" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D298" s="2"/>
       <c r="E298" s="2"/>
@@ -11809,7 +11815,7 @@
     </row>
     <row r="299" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A299" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B299" s="4"/>
       <c r="C299" s="4"/>
@@ -11838,7 +11844,7 @@
     </row>
     <row r="300" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A300" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B300" s="4"/>
       <c r="C300" s="4"/>
@@ -11867,7 +11873,7 @@
     </row>
     <row r="301" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A301" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B301" s="4"/>
       <c r="C301" s="4"/>
@@ -11896,7 +11902,7 @@
     </row>
     <row r="302" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A302" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B302" s="4"/>
       <c r="C302" s="4"/>
@@ -11925,7 +11931,7 @@
     </row>
     <row r="303" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A303" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B303" s="4"/>
       <c r="C303" s="4"/>
@@ -11954,10 +11960,10 @@
     </row>
     <row r="304" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A304" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="B304" s="4" t="s">
         <v>478</v>
-      </c>
-      <c r="B304" s="4" t="s">
-        <v>479</v>
       </c>
       <c r="C304" s="4"/>
       <c r="D304" s="2"/>
@@ -11985,7 +11991,7 @@
     </row>
     <row r="305" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A305" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B305" s="4"/>
       <c r="C305" s="4"/>
@@ -12014,11 +12020,11 @@
     </row>
     <row r="306" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A306" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B306" s="4"/>
       <c r="C306" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D306" s="2"/>
       <c r="E306" s="2"/>
@@ -12045,11 +12051,11 @@
     </row>
     <row r="307" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A307" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B307" s="4"/>
       <c r="C307" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D307" s="2"/>
       <c r="E307" s="2"/>
@@ -12076,11 +12082,11 @@
     </row>
     <row r="308" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A308" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B308" s="4"/>
       <c r="C308" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D308" s="2"/>
       <c r="E308" s="2"/>
@@ -12107,7 +12113,7 @@
     </row>
     <row r="309" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A309" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B309" s="4"/>
       <c r="C309" s="4"/>
@@ -12136,11 +12142,11 @@
     </row>
     <row r="310" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A310" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B310" s="4"/>
       <c r="C310" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D310" s="2"/>
       <c r="E310" s="2"/>
@@ -12167,7 +12173,7 @@
     </row>
     <row r="311" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A311" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B311" s="4"/>
       <c r="C311" s="4"/>
@@ -12196,11 +12202,11 @@
     </row>
     <row r="312" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A312" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B312" s="4"/>
       <c r="C312" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D312" s="2"/>
       <c r="E312" s="2"/>
@@ -12227,7 +12233,7 @@
     </row>
     <row r="313" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A313" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B313" s="4"/>
       <c r="C313" s="4"/>
@@ -12256,7 +12262,7 @@
     </row>
     <row r="314" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A314" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B314" s="4"/>
       <c r="C314" s="4"/>
@@ -12285,11 +12291,11 @@
     </row>
     <row r="315" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A315" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B315" s="4"/>
       <c r="C315" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D315" s="2"/>
       <c r="E315" s="2"/>
@@ -12316,7 +12322,7 @@
     </row>
     <row r="316" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A316" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B316" s="4"/>
       <c r="C316" s="4"/>
@@ -12345,11 +12351,11 @@
     </row>
     <row r="317" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A317" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B317" s="4"/>
       <c r="C317" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D317" s="2"/>
       <c r="E317" s="2"/>
@@ -12376,11 +12382,11 @@
     </row>
     <row r="318" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A318" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B318" s="4"/>
       <c r="C318" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D318" s="2"/>
       <c r="E318" s="2"/>
@@ -12407,7 +12413,7 @@
     </row>
     <row r="319" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A319" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B319" s="4"/>
       <c r="C319" s="4"/>
@@ -12436,11 +12442,11 @@
     </row>
     <row r="320" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A320" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B320" s="4"/>
       <c r="C320" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D320" s="2"/>
       <c r="E320" s="2"/>
@@ -12467,7 +12473,7 @@
     </row>
     <row r="321" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A321" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B321" s="4"/>
       <c r="C321" s="4"/>
@@ -12496,7 +12502,7 @@
     </row>
     <row r="322" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A322" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B322" s="4"/>
       <c r="C322" s="4"/>
@@ -12525,11 +12531,11 @@
     </row>
     <row r="323" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A323" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B323" s="4"/>
       <c r="C323" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D323" s="2"/>
       <c r="E323" s="2"/>
@@ -12556,7 +12562,7 @@
     </row>
     <row r="324" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A324" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B324" s="4"/>
       <c r="C324" s="4"/>
@@ -12585,7 +12591,7 @@
     </row>
     <row r="325" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A325" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B325" s="4"/>
       <c r="C325" s="4"/>
@@ -12614,11 +12620,11 @@
     </row>
     <row r="326" spans="1:25" ht="143" x14ac:dyDescent="0.15">
       <c r="A326" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B326" s="4"/>
       <c r="C326" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D326" s="2"/>
       <c r="E326" s="2"/>
@@ -12645,11 +12651,11 @@
     </row>
     <row r="327" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A327" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B327" s="4"/>
       <c r="C327" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D327" s="2"/>
       <c r="E327" s="2"/>
@@ -12676,7 +12682,7 @@
     </row>
     <row r="328" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A328" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B328" s="4"/>
       <c r="C328" s="4"/>
@@ -12705,11 +12711,11 @@
     </row>
     <row r="329" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A329" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B329" s="4"/>
       <c r="C329" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D329" s="2"/>
       <c r="E329" s="2"/>
@@ -12736,7 +12742,7 @@
     </row>
     <row r="330" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A330" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B330" s="4"/>
       <c r="D330" s="2"/>
@@ -12764,11 +12770,11 @@
     </row>
     <row r="331" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A331" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B331" s="4"/>
       <c r="C331" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D331" s="2"/>
       <c r="E331" s="2"/>
@@ -12795,11 +12801,11 @@
     </row>
     <row r="332" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A332" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B332" s="4"/>
       <c r="C332" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D332" s="2"/>
       <c r="E332" s="2"/>
@@ -12826,7 +12832,7 @@
     </row>
     <row r="333" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A333" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B333" s="4"/>
       <c r="C333" s="4"/>
@@ -12855,7 +12861,7 @@
     </row>
     <row r="334" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A334" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B334" s="4"/>
       <c r="C334" s="4"/>
@@ -12884,11 +12890,11 @@
     </row>
     <row r="335" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A335" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B335" s="4"/>
       <c r="C335" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D335" s="2"/>
       <c r="E335" s="2"/>
@@ -12915,7 +12921,7 @@
     </row>
     <row r="336" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A336" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B336" s="4"/>
       <c r="C336" s="4"/>
@@ -12944,7 +12950,7 @@
     </row>
     <row r="337" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A337" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B337" s="4"/>
       <c r="C337" s="4"/>
@@ -12973,11 +12979,11 @@
     </row>
     <row r="338" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A338" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B338" s="4"/>
       <c r="C338" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D338" s="2"/>
       <c r="E338" s="2"/>
@@ -13004,7 +13010,7 @@
     </row>
     <row r="339" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A339" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B339" s="4"/>
       <c r="C339" s="4"/>
@@ -13033,11 +13039,11 @@
     </row>
     <row r="340" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A340" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B340" s="4"/>
       <c r="C340" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D340" s="2"/>
       <c r="E340" s="2"/>
@@ -13064,7 +13070,7 @@
     </row>
     <row r="341" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A341" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B341" s="4"/>
       <c r="C341" s="4"/>
@@ -13093,10 +13099,10 @@
     </row>
     <row r="342" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A342" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B342" s="4" t="s">
         <v>535</v>
-      </c>
-      <c r="B342" s="4" t="s">
-        <v>536</v>
       </c>
       <c r="C342" s="4"/>
       <c r="D342" s="2"/>
@@ -13124,7 +13130,7 @@
     </row>
     <row r="343" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A343" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B343" s="4"/>
       <c r="C343" s="4"/>
@@ -13153,7 +13159,7 @@
     </row>
     <row r="344" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A344" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B344" s="4"/>
       <c r="C344" s="4"/>
@@ -13182,7 +13188,7 @@
     </row>
     <row r="345" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A345" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B345" s="4"/>
       <c r="C345" s="4"/>
@@ -13211,11 +13217,11 @@
     </row>
     <row r="346" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A346" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B346" s="4"/>
       <c r="C346" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D346" s="2"/>
       <c r="E346" s="2"/>
@@ -13242,11 +13248,11 @@
     </row>
     <row r="347" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A347" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B347" s="4"/>
       <c r="C347" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D347" s="2"/>
       <c r="E347" s="2"/>
@@ -13273,10 +13279,10 @@
     </row>
     <row r="348" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A348" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="B348" s="4" t="s">
         <v>544</v>
-      </c>
-      <c r="B348" s="4" t="s">
-        <v>545</v>
       </c>
       <c r="C348" s="4"/>
       <c r="D348" s="2"/>
@@ -13304,11 +13310,11 @@
     </row>
     <row r="349" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A349" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B349" s="4"/>
       <c r="C349" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D349" s="2"/>
       <c r="E349" s="2"/>
@@ -13335,7 +13341,7 @@
     </row>
     <row r="350" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A350" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B350" s="4"/>
       <c r="C350" s="4"/>
@@ -13364,11 +13370,11 @@
     </row>
     <row r="351" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A351" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B351" s="4"/>
       <c r="C351" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D351" s="2"/>
       <c r="E351" s="2"/>
@@ -13395,7 +13401,7 @@
     </row>
     <row r="352" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A352" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B352" s="4"/>
       <c r="C352" s="4"/>
@@ -13424,11 +13430,11 @@
     </row>
     <row r="353" spans="1:25" ht="143" x14ac:dyDescent="0.15">
       <c r="A353" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B353" s="4"/>
       <c r="C353" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D353" s="2"/>
       <c r="E353" s="2"/>
@@ -13455,10 +13461,10 @@
     </row>
     <row r="354" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A354" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="B354" s="4" t="s">
         <v>554</v>
-      </c>
-      <c r="B354" s="4" t="s">
-        <v>555</v>
       </c>
       <c r="C354" s="4"/>
       <c r="D354" s="2"/>
@@ -13486,11 +13492,11 @@
     </row>
     <row r="355" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A355" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B355" s="4"/>
       <c r="C355" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D355" s="2"/>
       <c r="E355" s="2"/>
@@ -13517,11 +13523,11 @@
     </row>
     <row r="356" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A356" s="4" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="B356" s="4"/>
       <c r="C356" s="4" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D356" s="2"/>
       <c r="E356" s="2"/>
@@ -13548,7 +13554,7 @@
     </row>
     <row r="357" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A357" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B357" s="4"/>
       <c r="C357" s="4"/>
@@ -13577,10 +13583,10 @@
     </row>
     <row r="358" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A358" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="B358" s="4" t="s">
         <v>559</v>
-      </c>
-      <c r="B358" s="4" t="s">
-        <v>560</v>
       </c>
       <c r="C358" s="4"/>
       <c r="D358" s="2"/>
@@ -13608,7 +13614,7 @@
     </row>
     <row r="359" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A359" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B359" s="4"/>
       <c r="C359" s="4"/>
@@ -13637,7 +13643,7 @@
     </row>
     <row r="360" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A360" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B360" s="4"/>
       <c r="C360" s="4"/>
@@ -13666,7 +13672,7 @@
     </row>
     <row r="361" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A361" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B361" s="4"/>
       <c r="C361" s="4"/>
@@ -13695,10 +13701,10 @@
     </row>
     <row r="362" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A362" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="B362" s="4" t="s">
         <v>564</v>
-      </c>
-      <c r="B362" s="4" t="s">
-        <v>565</v>
       </c>
       <c r="C362" s="4"/>
       <c r="D362" s="2"/>
@@ -13726,10 +13732,10 @@
     </row>
     <row r="363" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A363" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="B363" s="4" t="s">
         <v>566</v>
-      </c>
-      <c r="B363" s="4" t="s">
-        <v>567</v>
       </c>
       <c r="C363" s="4"/>
       <c r="D363" s="2"/>
@@ -13757,10 +13763,10 @@
     </row>
     <row r="364" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A364" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="B364" s="4" t="s">
         <v>568</v>
-      </c>
-      <c r="B364" s="4" t="s">
-        <v>569</v>
       </c>
       <c r="C364" s="4"/>
       <c r="D364" s="2"/>
@@ -13788,11 +13794,11 @@
     </row>
     <row r="365" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A365" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B365" s="4"/>
       <c r="C365" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D365" s="2"/>
       <c r="E365" s="2"/>
@@ -13819,7 +13825,7 @@
     </row>
     <row r="366" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A366" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B366" s="4"/>
       <c r="C366" s="4"/>
@@ -13848,7 +13854,7 @@
     </row>
     <row r="367" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A367" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B367" s="4"/>
       <c r="C367" s="4"/>
@@ -13877,7 +13883,7 @@
     </row>
     <row r="368" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A368" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B368" s="4"/>
       <c r="C368" s="4"/>
@@ -13906,7 +13912,7 @@
     </row>
     <row r="369" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A369" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B369" s="4"/>
       <c r="C369" s="4"/>
@@ -13935,11 +13941,11 @@
     </row>
     <row r="370" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A370" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B370" s="4"/>
       <c r="C370" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D370" s="2"/>
       <c r="E370" s="2"/>
@@ -13966,7 +13972,7 @@
     </row>
     <row r="371" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A371" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B371" s="4"/>
       <c r="C371" s="4"/>
@@ -13995,10 +14001,10 @@
     </row>
     <row r="372" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A372" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="B372" s="4" t="s">
         <v>579</v>
-      </c>
-      <c r="B372" s="4" t="s">
-        <v>580</v>
       </c>
       <c r="C372" s="4"/>
       <c r="D372" s="2"/>
@@ -14026,7 +14032,7 @@
     </row>
     <row r="373" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A373" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B373" s="4"/>
       <c r="C373" s="4"/>
@@ -14055,7 +14061,7 @@
     </row>
     <row r="374" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A374" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B374" s="4"/>
       <c r="C374" s="4"/>
@@ -14084,7 +14090,7 @@
     </row>
     <row r="375" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A375" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B375" s="4"/>
       <c r="C375" s="4"/>
@@ -14113,10 +14119,10 @@
     </row>
     <row r="376" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A376" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="B376" s="4" t="s">
         <v>584</v>
-      </c>
-      <c r="B376" s="4" t="s">
-        <v>585</v>
       </c>
       <c r="C376" s="4"/>
       <c r="D376" s="2"/>
@@ -14144,10 +14150,10 @@
     </row>
     <row r="377" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A377" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="B377" s="4" t="s">
         <v>586</v>
-      </c>
-      <c r="B377" s="4" t="s">
-        <v>587</v>
       </c>
       <c r="C377" s="4"/>
       <c r="D377" s="2"/>
@@ -14175,10 +14181,10 @@
     </row>
     <row r="378" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A378" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="B378" s="4" t="s">
         <v>588</v>
-      </c>
-      <c r="B378" s="4" t="s">
-        <v>589</v>
       </c>
       <c r="C378" s="4"/>
       <c r="D378" s="2"/>
@@ -14206,11 +14212,11 @@
     </row>
     <row r="379" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A379" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B379" s="4"/>
       <c r="C379" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D379" s="2"/>
       <c r="E379" s="2"/>
@@ -14237,13 +14243,13 @@
     </row>
     <row r="380" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A380" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="B380" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="B380" s="4" t="s">
+      <c r="C380" s="4" t="s">
         <v>593</v>
-      </c>
-      <c r="C380" s="4" t="s">
-        <v>594</v>
       </c>
       <c r="D380" s="2"/>
       <c r="E380" s="2"/>
@@ -14270,11 +14276,11 @@
     </row>
     <row r="381" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A381" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B381" s="4"/>
       <c r="C381" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D381" s="2"/>
       <c r="E381" s="2"/>
@@ -14301,7 +14307,7 @@
     </row>
     <row r="382" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A382" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B382" s="4"/>
       <c r="C382" s="4"/>
@@ -14330,11 +14336,11 @@
     </row>
     <row r="383" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A383" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B383" s="4"/>
       <c r="C383" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D383" s="2"/>
       <c r="E383" s="2"/>
@@ -14361,11 +14367,11 @@
     </row>
     <row r="384" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A384" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B384" s="4"/>
       <c r="C384" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D384" s="2"/>
       <c r="E384" s="2"/>
@@ -14392,10 +14398,10 @@
     </row>
     <row r="385" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A385" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="B385" s="4" t="s">
         <v>602</v>
-      </c>
-      <c r="B385" s="4" t="s">
-        <v>603</v>
       </c>
       <c r="C385" s="4"/>
       <c r="D385" s="2"/>
@@ -14423,11 +14429,11 @@
     </row>
     <row r="386" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A386" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B386" s="4"/>
       <c r="C386" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D386" s="2"/>
       <c r="E386" s="2"/>
@@ -14454,11 +14460,11 @@
     </row>
     <row r="387" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A387" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B387" s="4"/>
       <c r="C387" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D387" s="2"/>
       <c r="E387" s="2"/>
@@ -14485,7 +14491,7 @@
     </row>
     <row r="388" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A388" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B388" s="4"/>
       <c r="C388" s="4"/>
@@ -14512,9 +14518,9 @@
       <c r="X388" s="2"/>
       <c r="Y388" s="2"/>
     </row>
-    <row r="389" spans="1:25" ht="13" x14ac:dyDescent="0.15">
-      <c r="A389" s="4" t="s">
-        <v>609</v>
+    <row r="389" spans="1:25" ht="16" x14ac:dyDescent="0.25">
+      <c r="A389" s="7" t="s">
+        <v>667</v>
       </c>
       <c r="B389" s="4"/>
       <c r="C389" s="4"/>
@@ -14543,7 +14549,7 @@
     </row>
     <row r="390" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A390" s="4" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B390" s="4"/>
       <c r="C390" s="4"/>
@@ -14572,10 +14578,10 @@
     </row>
     <row r="391" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A391" s="4" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B391" s="4" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C391" s="4"/>
       <c r="D391" s="2"/>
@@ -14603,11 +14609,11 @@
     </row>
     <row r="392" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A392" s="4" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B392" s="4"/>
       <c r="C392" s="4" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D392" s="2"/>
       <c r="E392" s="2"/>
@@ -14634,11 +14640,11 @@
     </row>
     <row r="393" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A393" s="4" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B393" s="4"/>
       <c r="C393" s="4" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D393" s="2"/>
       <c r="E393" s="2"/>
@@ -14665,10 +14671,10 @@
     </row>
     <row r="394" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A394" s="4" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B394" s="4" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C394" s="4"/>
       <c r="D394" s="2"/>
@@ -14696,11 +14702,11 @@
     </row>
     <row r="395" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A395" s="4" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B395" s="4"/>
       <c r="C395" s="4" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D395" s="2"/>
       <c r="E395" s="2"/>
@@ -14727,11 +14733,11 @@
     </row>
     <row r="396" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A396" s="4" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B396" s="4"/>
       <c r="C396" s="4" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D396" s="2"/>
       <c r="E396" s="2"/>
@@ -14758,11 +14764,11 @@
     </row>
     <row r="397" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A397" s="4" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B397" s="4"/>
       <c r="C397" s="4" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D397" s="2"/>
       <c r="E397" s="2"/>
@@ -14789,10 +14795,10 @@
     </row>
     <row r="398" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A398" s="4" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B398" s="4" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C398" s="4"/>
       <c r="D398" s="2"/>
@@ -14820,7 +14826,7 @@
     </row>
     <row r="399" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A399" s="4" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B399" s="4"/>
       <c r="C399" s="4"/>
@@ -14849,11 +14855,11 @@
     </row>
     <row r="400" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A400" s="4" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B400" s="4"/>
       <c r="C400" s="4" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D400" s="2"/>
       <c r="E400" s="2"/>
@@ -14880,10 +14886,10 @@
     </row>
     <row r="401" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A401" s="4" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B401" s="4" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C401" s="4"/>
       <c r="D401" s="2"/>
@@ -14911,11 +14917,11 @@
     </row>
     <row r="402" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A402" s="4" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B402" s="4"/>
       <c r="C402" s="4" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D402" s="2"/>
       <c r="E402" s="2"/>
@@ -14942,7 +14948,7 @@
     </row>
     <row r="403" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A403" s="4" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B403" s="4"/>
       <c r="C403" s="4"/>
@@ -14971,7 +14977,7 @@
     </row>
     <row r="404" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A404" s="4" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B404" s="4"/>
       <c r="C404" s="4"/>
@@ -15000,11 +15006,11 @@
     </row>
     <row r="405" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A405" s="4" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B405" s="4"/>
       <c r="C405" s="4" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D405" s="2"/>
       <c r="E405" s="2"/>
@@ -15031,7 +15037,7 @@
     </row>
     <row r="406" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A406" s="4" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B406" s="4"/>
       <c r="C406" s="4"/>
@@ -15060,11 +15066,11 @@
     </row>
     <row r="407" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A407" s="4" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B407" s="4"/>
       <c r="C407" s="4" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D407" s="2"/>
       <c r="E407" s="2"/>
@@ -15091,7 +15097,7 @@
     </row>
     <row r="408" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A408" s="4" t="s">
-        <v>641</v>
+        <v>668</v>
       </c>
       <c r="B408" s="4"/>
       <c r="C408" s="4"/>
@@ -15120,7 +15126,7 @@
     </row>
     <row r="409" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A409" s="4" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="B409" s="4"/>
       <c r="C409" s="4"/>
@@ -15149,7 +15155,7 @@
     </row>
     <row r="410" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A410" s="4" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="B410" s="4"/>
       <c r="C410" s="4"/>
@@ -15178,7 +15184,7 @@
     </row>
     <row r="411" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A411" s="4" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="B411" s="4"/>
       <c r="C411" s="4"/>
@@ -15207,10 +15213,10 @@
     </row>
     <row r="412" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A412" s="4" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="B412" s="4" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="C412" s="4"/>
       <c r="D412" s="2"/>
@@ -15238,7 +15244,7 @@
     </row>
     <row r="413" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A413" s="4" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="B413" s="4"/>
       <c r="C413" s="4"/>
@@ -15267,7 +15273,7 @@
     </row>
     <row r="414" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A414" s="4" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="B414" s="4"/>
       <c r="C414" s="4"/>
@@ -15296,7 +15302,7 @@
     </row>
     <row r="415" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A415" s="4" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="B415" s="4"/>
       <c r="C415" s="4"/>
@@ -15325,7 +15331,7 @@
     </row>
     <row r="416" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A416" s="4" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="B416" s="4"/>
       <c r="C416" s="4"/>
@@ -15354,7 +15360,7 @@
     </row>
     <row r="417" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A417" s="4" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="B417" s="4"/>
       <c r="C417" s="4"/>
@@ -15383,7 +15389,7 @@
     </row>
     <row r="418" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A418" s="4" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B418" s="4"/>
       <c r="C418" s="2"/>
@@ -15412,7 +15418,7 @@
     </row>
     <row r="419" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A419" s="4" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="B419" s="4"/>
       <c r="C419" s="2"/>
@@ -15441,7 +15447,7 @@
     </row>
     <row r="420" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A420" s="4" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="B420" s="4"/>
       <c r="C420" s="2"/>
@@ -15470,10 +15476,10 @@
     </row>
     <row r="421" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A421" s="4" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="B421" s="4" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="C421" s="2"/>
       <c r="D421" s="2"/>

</xml_diff>

<commit_message>
Update wikipathways changing names everyday
</commit_message>
<xml_diff>
--- a/mappings/wikipathways_reactome.xlsx
+++ b/mappings/wikipathways_reactome.xlsx
@@ -1841,7 +1841,7 @@
     <t xml:space="preserve">RAC1/PAK1/p38/MMP2 Pathway</t>
   </si>
   <si>
-    <t xml:space="preserve">p38MAPK events isPartOf Rac1/Pak1/p38/MMP-2 pathway*</t>
+    <t xml:space="preserve">p38MAPK events isPartOf RAC1/PAK1/p38/MMP2 Pathway*</t>
   </si>
   <si>
     <t xml:space="preserve">RalA downstream regulated genes</t>
@@ -2569,16 +2569,16 @@
   <dimension ref="A1:Y421"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A307" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A313" activeCellId="0" sqref="A313"/>
+      <selection pane="topLeft" activeCell="B312" activeCellId="0" sqref="B312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="70.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="55.8877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="61.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="69.9234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="55.2091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="61.015306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11981,7 +11981,7 @@
       <c r="X311" s="3"/>
       <c r="Y311" s="3"/>
     </row>
-    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="4" t="s">
         <v>502</v>
       </c>

</xml_diff>